<commit_message>
added my pick to signup sheet
</commit_message>
<xml_diff>
--- a/_signup_sheet/30 Days of Mapping Sign-up.xlsx
+++ b/_signup_sheet/30 Days of Mapping Sign-up.xlsx
@@ -100,9 +100,6 @@
     <t>Challenge yourself to use the fewest possible elements (color, line weight, labels) while keeping the map clear, useful, and informative.</t>
   </si>
   <si>
-    <t>a</t>
-  </si>
-  <si>
     <t>Map from 2125</t>
   </si>
   <si>
@@ -179,6 +176,9 @@
   </si>
   <si>
     <t>Focus on toponymy (place names). Experiment with font choices, label placement, typography, multiple languages, or the history and meaning behind a name.</t>
+  </si>
+  <si>
+    <t>@pendulating</t>
   </si>
   <si>
     <t>Hexagons</t>
@@ -749,19 +749,16 @@
       <c r="C13" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="E13" s="16" t="s">
-        <v>29</v>
-      </c>
     </row>
     <row r="14">
       <c r="A14" s="13">
         <v>45973.0</v>
       </c>
       <c r="B14" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="15" t="s">
         <v>30</v>
-      </c>
-      <c r="C14" s="15" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="15">
@@ -769,10 +766,10 @@
         <v>45974.0</v>
       </c>
       <c r="B15" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" s="15" t="s">
         <v>32</v>
-      </c>
-      <c r="C15" s="15" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="16">
@@ -780,10 +777,10 @@
         <v>45975.0</v>
       </c>
       <c r="B16" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="15" t="s">
         <v>34</v>
-      </c>
-      <c r="C16" s="15" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="17">
@@ -791,10 +788,10 @@
         <v>45976.0</v>
       </c>
       <c r="B17" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" s="15" t="s">
         <v>36</v>
-      </c>
-      <c r="C17" s="15" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="18">
@@ -802,10 +799,10 @@
         <v>45977.0</v>
       </c>
       <c r="B18" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" s="15" t="s">
         <v>38</v>
-      </c>
-      <c r="C18" s="15" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="19">
@@ -813,10 +810,10 @@
         <v>45978.0</v>
       </c>
       <c r="B19" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="C19" s="15" t="s">
         <v>40</v>
-      </c>
-      <c r="C19" s="15" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="20">
@@ -824,10 +821,10 @@
         <v>45979.0</v>
       </c>
       <c r="B20" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20" s="15" t="s">
         <v>42</v>
-      </c>
-      <c r="C20" s="15" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="21">
@@ -835,10 +832,10 @@
         <v>45980.0</v>
       </c>
       <c r="B21" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="C21" s="15" t="s">
         <v>44</v>
-      </c>
-      <c r="C21" s="15" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="22">
@@ -846,10 +843,10 @@
         <v>45981.0</v>
       </c>
       <c r="B22" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="C22" s="15" t="s">
         <v>46</v>
-      </c>
-      <c r="C22" s="15" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="23">
@@ -857,10 +854,10 @@
         <v>45982.0</v>
       </c>
       <c r="B23" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="C23" s="15" t="s">
         <v>48</v>
-      </c>
-      <c r="C23" s="15" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="24">
@@ -868,10 +865,10 @@
         <v>45983.0</v>
       </c>
       <c r="B24" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="C24" s="15" t="s">
         <v>50</v>
-      </c>
-      <c r="C24" s="15" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="25">
@@ -879,10 +876,10 @@
         <v>45984.0</v>
       </c>
       <c r="B25" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="C25" s="15" t="s">
         <v>52</v>
-      </c>
-      <c r="C25" s="15" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="26">
@@ -890,9 +887,12 @@
         <v>45985.0</v>
       </c>
       <c r="B26" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="C26" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="C26" s="15" t="s">
+      <c r="D26" s="16" t="s">
         <v>55</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated signup sheet with responses up to today nov 1
</commit_message>
<xml_diff>
--- a/_signup_sheet/30 Days of Mapping Sign-up.xlsx
+++ b/_signup_sheet/30 Days of Mapping Sign-up.xlsx
@@ -11,9 +11,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="68">
-  <si>
-    <t>Sign up here! Enter your GitHub username (i.e., @pendulating). In case you aren't familiar with GitHub and plan to just submit your finished map, you can also just put your full name.</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="86">
+  <si>
+    <t>Sign up here! Enter your GitHub username (i.e., @gsagostini) so we can add you to the 30DoM repository. In case you aren't familiar with GitHub and would like to submit your finished map to us directly, you can also just put your full name.</t>
+  </si>
+  <si>
+    <t>Sent email?</t>
   </si>
   <si>
     <t>Date</t>
@@ -40,6 +43,15 @@
     <t>Challenge Classic: Map with point data (e.g., individual locations, points of interest, clusters). Focus on effective symbolization and density visualization.</t>
   </si>
   <si>
+    <t>@chae-won-lee</t>
+  </si>
+  <si>
+    <t>@amyxqc</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
     <t>Lines</t>
   </si>
   <si>
@@ -52,12 +64,24 @@
     <t>Challenge Classic: Create a map focused on area features (e.g., administrative regions, land use, boundaries). Use fills, patterns, and choropleth techniques.</t>
   </si>
   <si>
+    <t>@Navxihziq</t>
+  </si>
+  <si>
     <t>Data challenge: My Data</t>
   </si>
   <si>
     <t>Map something personal using your own dataset. Visualize GPS traces, your commute, or a unique, small dataset you created. (Need simple data? Try geojson.io)</t>
   </si>
   <si>
+    <t>@gsagostini</t>
+  </si>
+  <si>
+    <t>@pendulating</t>
+  </si>
+  <si>
+    <t>@jennah-gosciak</t>
+  </si>
+  <si>
     <t>Earth</t>
   </si>
   <si>
@@ -88,18 +112,30 @@
     <t>Step away from the screen! Create your map using traditional methods (e.g., pen, pencil, paint, collage, physical models). Show the handmade process!</t>
   </si>
   <si>
+    <t>@annaloganmc</t>
+  </si>
+  <si>
+    <t>@tqueer (would love to collaborate / co-work!)</t>
+  </si>
+  <si>
     <t>Air</t>
   </si>
   <si>
     <t>Classical Elements 2/4: Focus on the atmosphere. Map weather, wind patterns, air traffic, pollution, or airborne transmission (e.g., pollen, sound).</t>
   </si>
   <si>
+    <t>@jfinocchiaro</t>
+  </si>
+  <si>
     <t>Minimal map</t>
   </si>
   <si>
     <t>Challenge yourself to use the fewest possible elements (color, line weight, labels) while keeping the map clear, useful, and informative.</t>
   </si>
   <si>
+    <t>@kennylpeng</t>
+  </si>
+  <si>
     <t>Map from 2125</t>
   </si>
   <si>
@@ -112,6 +148,9 @@
     <t>Start the timer! The maximum allowed time to design and produce this map is 10 minutes. Focus on speed, simplicity, and core communication.</t>
   </si>
   <si>
+    <t>@atmikapai13</t>
+  </si>
+  <si>
     <t>Data challenge: OpenStreetMap</t>
   </si>
   <si>
@@ -124,6 +163,9 @@
     <t>Classical Elements ¾: Focus on energy, light, or transformation. Map heat, wildfires, energy consumption, population density at night, or volcanic activity.</t>
   </si>
   <si>
+    <t>@simanirakiza</t>
+  </si>
+  <si>
     <t>Cell</t>
   </si>
   <si>
@@ -136,12 +178,18 @@
     <t>Challenge Classic: Experimentation is key! Create your map using a software, language, library, or technique you have never used before.</t>
   </si>
   <si>
+    <t>Jessica Spencer</t>
+  </si>
+  <si>
     <t>Out of this world</t>
   </si>
   <si>
     <t>Map something non-Earth: a fantasy realm, an exoplanet, the Moon, Mars, deep space, or a purely conceptual place (e.g., a mental map).</t>
   </si>
   <si>
+    <t>@appelson</t>
+  </si>
+  <si>
     <t>Projections</t>
   </si>
   <si>
@@ -172,15 +220,15 @@
     <t>Show how you make a map. This could be a tutorial, a step-by-step graphic, a blog post, a video, or a screenshot of your work environment. Combine it with a map from another day!</t>
   </si>
   <si>
+    <t>@shuvom-s</t>
+  </si>
+  <si>
     <t>Places and their names</t>
   </si>
   <si>
     <t>Focus on toponymy (place names). Experiment with font choices, label placement, typography, multiple languages, or the history and meaning behind a name.</t>
   </si>
   <si>
-    <t>@pendulating</t>
-  </si>
-  <si>
     <t>Hexagons</t>
   </si>
   <si>
@@ -193,6 +241,9 @@
     <t>(World Sustainable Transport Day) Map mobility, traffic flow, public transit networks, logistics chains, or advocate for sustainable transport options.</t>
   </si>
   <si>
+    <t>Not to volunteer jhilleary@mbta.com, but he might be interested!</t>
+  </si>
+  <si>
     <t>Boundaries</t>
   </si>
   <si>
@@ -203,6 +254,9 @@
   </si>
   <si>
     <t>(Black Friday) Interpret the theme of Black. The map can be purely monochromatic, represent absence/darkness (e.g., light pollution), or relate to themes of consumption.</t>
+  </si>
+  <si>
+    <t>@sidhikabalachandar</t>
   </si>
   <si>
     <t>Raster</t>
@@ -224,7 +278,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm-dd-yyyy"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -246,6 +300,11 @@
     </font>
     <font/>
     <font>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -253,6 +312,7 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
@@ -325,7 +385,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -344,36 +404,39 @@
     <xf borderId="3" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="6" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="7" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="5" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="6" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="7" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -597,6 +660,7 @@
     <col customWidth="1" min="4" max="4" width="25.25"/>
     <col customWidth="1" min="5" max="5" width="25.5"/>
     <col customWidth="1" min="6" max="6" width="25.38"/>
+    <col customWidth="1" min="7" max="7" width="50.0"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -608,3271 +672,3387 @@
       </c>
       <c r="E1" s="5"/>
       <c r="F1" s="6"/>
+      <c r="H1" s="7" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="8" t="s">
+      <c r="A2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="B2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="C2" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="D2" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="E2" s="12" t="s">
         <v>6</v>
       </c>
+      <c r="F2" s="13" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="3">
-      <c r="A3" s="13">
+      <c r="A3" s="14">
         <v>45962.0</v>
       </c>
-      <c r="B3" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="15" t="s">
+      <c r="B3" s="15" t="s">
         <v>8</v>
       </c>
+      <c r="C3" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="4">
-      <c r="A4" s="13">
+      <c r="A4" s="14">
         <v>45963.0</v>
       </c>
-      <c r="B4" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="15" t="s">
+      <c r="B4" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="7"/>
+      <c r="H4" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="14">
+        <v>45964.0</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="14">
+        <v>45965.0</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="14">
+        <v>45966.0</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="14">
+        <v>45967.0</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="14">
+        <v>45968.0</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="14">
+        <v>45969.0</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="7" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="13">
-        <v>45964.0</v>
-      </c>
-      <c r="B5" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="15" t="s">
+      <c r="H10" s="7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="13">
-        <v>45965.0</v>
-      </c>
-      <c r="B6" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="15" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="13">
-        <v>45966.0</v>
-      </c>
-      <c r="B7" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" s="15" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="13">
-        <v>45967.0</v>
-      </c>
-      <c r="B8" s="14" t="s">
+    <row r="11">
+      <c r="A11" s="14">
+        <v>45970.0</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="14">
+        <v>45971.0</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="14">
+        <v>45972.0</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="14">
+        <v>45973.0</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="15" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="13">
-        <v>45968.0</v>
-      </c>
-      <c r="B9" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" s="15" t="s">
+    </row>
+    <row r="15">
+      <c r="A15" s="14">
+        <v>45974.0</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="14">
+        <v>45975.0</v>
+      </c>
+      <c r="B16" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="14">
+        <v>45976.0</v>
+      </c>
+      <c r="B17" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="C17" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="14">
+        <v>45977.0</v>
+      </c>
+      <c r="B18" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="C18" s="16" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="14">
+        <v>45978.0</v>
+      </c>
+      <c r="B19" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="C19" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="D19" s="17" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="14">
+        <v>45979.0</v>
+      </c>
+      <c r="B20" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="C20" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="14">
+        <v>45980.0</v>
+      </c>
+      <c r="B21" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="C21" s="16" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="14">
+        <v>45981.0</v>
+      </c>
+      <c r="B22" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="C22" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="14">
+        <v>45982.0</v>
+      </c>
+      <c r="B23" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="C23" s="16" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="14">
+        <v>45983.0</v>
+      </c>
+      <c r="B24" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="C24" s="16" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="14">
+        <v>45984.0</v>
+      </c>
+      <c r="B25" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="C25" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="14">
+        <v>45985.0</v>
+      </c>
+      <c r="B26" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="C26" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="14">
+        <v>45986.0</v>
+      </c>
+      <c r="B27" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="C27" s="16" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="14">
+        <v>45987.0</v>
+      </c>
+      <c r="B28" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="C28" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G28" s="17" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="14">
+        <v>45988.0</v>
+      </c>
+      <c r="B29" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="C29" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="14">
+        <v>45989.0</v>
+      </c>
+      <c r="B30" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="C30" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="14">
+        <v>45990.0</v>
+      </c>
+      <c r="B31" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="C31" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="D31" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E31" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="14">
+        <v>45991.0</v>
+      </c>
+      <c r="B32" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="C32" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="D32" s="7" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" s="13">
-        <v>45969.0</v>
-      </c>
-      <c r="B10" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" s="15" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="13">
-        <v>45970.0</v>
-      </c>
-      <c r="B11" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" s="15" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="13">
-        <v>45971.0</v>
-      </c>
-      <c r="B12" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="C12" s="15" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="13">
-        <v>45972.0</v>
-      </c>
-      <c r="B13" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="C13" s="15" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="13">
-        <v>45973.0</v>
-      </c>
-      <c r="B14" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="C14" s="15" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="13">
-        <v>45974.0</v>
-      </c>
-      <c r="B15" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="C15" s="15" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="13">
-        <v>45975.0</v>
-      </c>
-      <c r="B16" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="C16" s="15" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="13">
-        <v>45976.0</v>
-      </c>
-      <c r="B17" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="C17" s="15" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="13">
-        <v>45977.0</v>
-      </c>
-      <c r="B18" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="C18" s="15" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="13">
-        <v>45978.0</v>
-      </c>
-      <c r="B19" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="C19" s="15" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="13">
-        <v>45979.0</v>
-      </c>
-      <c r="B20" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="C20" s="15" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="13">
-        <v>45980.0</v>
-      </c>
-      <c r="B21" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="C21" s="15" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="13">
-        <v>45981.0</v>
-      </c>
-      <c r="B22" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="C22" s="15" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="13">
-        <v>45982.0</v>
-      </c>
-      <c r="B23" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="C23" s="15" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="13">
-        <v>45983.0</v>
-      </c>
-      <c r="B24" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="C24" s="15" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="13">
-        <v>45984.0</v>
-      </c>
-      <c r="B25" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="C25" s="15" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="13">
-        <v>45985.0</v>
-      </c>
-      <c r="B26" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="C26" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="D26" s="16" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" s="13">
-        <v>45986.0</v>
-      </c>
-      <c r="B27" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="C27" s="15" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" s="13">
-        <v>45987.0</v>
-      </c>
-      <c r="B28" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="C28" s="15" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" s="13">
-        <v>45988.0</v>
-      </c>
-      <c r="B29" s="14" t="s">
-        <v>60</v>
-      </c>
-      <c r="C29" s="15" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" s="13">
-        <v>45989.0</v>
-      </c>
-      <c r="B30" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="C30" s="15" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" s="13">
-        <v>45990.0</v>
-      </c>
-      <c r="B31" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="C31" s="15" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" s="13">
-        <v>45991.0</v>
-      </c>
-      <c r="B32" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="C32" s="15" t="s">
-        <v>67</v>
-      </c>
-    </row>
     <row r="33">
-      <c r="B33" s="17"/>
+      <c r="B33" s="18"/>
     </row>
     <row r="34">
-      <c r="B34" s="17"/>
+      <c r="B34" s="18"/>
     </row>
     <row r="35">
-      <c r="B35" s="17"/>
+      <c r="B35" s="18"/>
     </row>
     <row r="36">
-      <c r="B36" s="17"/>
+      <c r="B36" s="18"/>
     </row>
     <row r="37">
-      <c r="B37" s="17"/>
+      <c r="B37" s="18"/>
     </row>
     <row r="38">
-      <c r="B38" s="17"/>
+      <c r="B38" s="18"/>
     </row>
     <row r="39">
-      <c r="B39" s="17"/>
+      <c r="B39" s="18"/>
     </row>
     <row r="40">
-      <c r="B40" s="17"/>
+      <c r="B40" s="18"/>
     </row>
     <row r="41">
-      <c r="B41" s="17"/>
+      <c r="B41" s="18"/>
     </row>
     <row r="42">
-      <c r="B42" s="17"/>
+      <c r="B42" s="18"/>
     </row>
     <row r="43">
-      <c r="B43" s="17"/>
+      <c r="B43" s="18"/>
     </row>
     <row r="44">
-      <c r="B44" s="17"/>
+      <c r="B44" s="18"/>
     </row>
     <row r="45">
-      <c r="B45" s="17"/>
+      <c r="B45" s="18"/>
     </row>
     <row r="46">
-      <c r="B46" s="17"/>
+      <c r="B46" s="18"/>
     </row>
     <row r="47">
-      <c r="B47" s="17"/>
+      <c r="B47" s="18"/>
     </row>
     <row r="48">
-      <c r="B48" s="17"/>
+      <c r="B48" s="18"/>
     </row>
     <row r="49">
-      <c r="B49" s="17"/>
+      <c r="B49" s="18"/>
     </row>
     <row r="50">
-      <c r="B50" s="17"/>
+      <c r="B50" s="18"/>
     </row>
     <row r="51">
-      <c r="B51" s="17"/>
+      <c r="B51" s="18"/>
     </row>
     <row r="52">
-      <c r="B52" s="17"/>
+      <c r="B52" s="18"/>
     </row>
     <row r="53">
-      <c r="B53" s="17"/>
+      <c r="B53" s="18"/>
     </row>
     <row r="54">
-      <c r="B54" s="17"/>
+      <c r="B54" s="18"/>
     </row>
     <row r="55">
-      <c r="B55" s="17"/>
+      <c r="B55" s="18"/>
     </row>
     <row r="56">
-      <c r="B56" s="17"/>
+      <c r="B56" s="18"/>
     </row>
     <row r="57">
-      <c r="B57" s="17"/>
+      <c r="B57" s="18"/>
     </row>
     <row r="58">
-      <c r="B58" s="17"/>
+      <c r="B58" s="18"/>
     </row>
     <row r="59">
-      <c r="B59" s="17"/>
+      <c r="B59" s="18"/>
     </row>
     <row r="60">
-      <c r="B60" s="17"/>
+      <c r="B60" s="18"/>
     </row>
     <row r="61">
-      <c r="B61" s="17"/>
+      <c r="B61" s="18"/>
     </row>
     <row r="62">
-      <c r="B62" s="17"/>
+      <c r="B62" s="18"/>
     </row>
     <row r="63">
-      <c r="B63" s="17"/>
+      <c r="B63" s="18"/>
     </row>
     <row r="64">
-      <c r="B64" s="17"/>
+      <c r="B64" s="18"/>
     </row>
     <row r="65">
-      <c r="B65" s="17"/>
+      <c r="B65" s="18"/>
     </row>
     <row r="66">
-      <c r="B66" s="17"/>
+      <c r="B66" s="18"/>
     </row>
     <row r="67">
-      <c r="B67" s="17"/>
+      <c r="B67" s="18"/>
     </row>
     <row r="68">
-      <c r="B68" s="17"/>
+      <c r="B68" s="18"/>
     </row>
     <row r="69">
-      <c r="B69" s="17"/>
+      <c r="B69" s="18"/>
     </row>
     <row r="70">
-      <c r="B70" s="17"/>
+      <c r="B70" s="18"/>
     </row>
     <row r="71">
-      <c r="B71" s="17"/>
+      <c r="B71" s="18"/>
     </row>
     <row r="72">
-      <c r="B72" s="17"/>
+      <c r="B72" s="18"/>
     </row>
     <row r="73">
-      <c r="B73" s="17"/>
+      <c r="B73" s="18"/>
     </row>
     <row r="74">
-      <c r="B74" s="17"/>
+      <c r="B74" s="18"/>
     </row>
     <row r="75">
-      <c r="B75" s="17"/>
+      <c r="B75" s="18"/>
     </row>
     <row r="76">
-      <c r="B76" s="17"/>
+      <c r="B76" s="18"/>
     </row>
     <row r="77">
-      <c r="B77" s="17"/>
+      <c r="B77" s="18"/>
     </row>
     <row r="78">
-      <c r="B78" s="17"/>
+      <c r="B78" s="18"/>
     </row>
     <row r="79">
-      <c r="B79" s="17"/>
+      <c r="B79" s="18"/>
     </row>
     <row r="80">
-      <c r="B80" s="17"/>
+      <c r="B80" s="18"/>
     </row>
     <row r="81">
-      <c r="B81" s="17"/>
+      <c r="B81" s="18"/>
     </row>
     <row r="82">
-      <c r="B82" s="17"/>
+      <c r="B82" s="18"/>
     </row>
     <row r="83">
-      <c r="B83" s="17"/>
+      <c r="B83" s="18"/>
     </row>
     <row r="84">
-      <c r="B84" s="17"/>
+      <c r="B84" s="18"/>
     </row>
     <row r="85">
-      <c r="B85" s="17"/>
+      <c r="B85" s="18"/>
     </row>
     <row r="86">
-      <c r="B86" s="17"/>
+      <c r="B86" s="18"/>
     </row>
     <row r="87">
-      <c r="B87" s="17"/>
+      <c r="B87" s="18"/>
     </row>
     <row r="88">
-      <c r="B88" s="17"/>
+      <c r="B88" s="18"/>
     </row>
     <row r="89">
-      <c r="B89" s="17"/>
+      <c r="B89" s="18"/>
     </row>
     <row r="90">
-      <c r="B90" s="17"/>
+      <c r="B90" s="18"/>
     </row>
     <row r="91">
-      <c r="B91" s="17"/>
+      <c r="B91" s="18"/>
     </row>
     <row r="92">
-      <c r="B92" s="17"/>
+      <c r="B92" s="18"/>
     </row>
     <row r="93">
-      <c r="B93" s="17"/>
+      <c r="B93" s="18"/>
     </row>
     <row r="94">
-      <c r="B94" s="17"/>
+      <c r="B94" s="18"/>
     </row>
     <row r="95">
-      <c r="B95" s="17"/>
+      <c r="B95" s="18"/>
     </row>
     <row r="96">
-      <c r="B96" s="17"/>
+      <c r="B96" s="18"/>
     </row>
     <row r="97">
-      <c r="B97" s="17"/>
+      <c r="B97" s="18"/>
     </row>
     <row r="98">
-      <c r="B98" s="17"/>
+      <c r="B98" s="18"/>
     </row>
     <row r="99">
-      <c r="B99" s="17"/>
+      <c r="B99" s="18"/>
     </row>
     <row r="100">
-      <c r="B100" s="17"/>
+      <c r="B100" s="18"/>
     </row>
     <row r="101">
-      <c r="B101" s="17"/>
+      <c r="B101" s="18"/>
     </row>
     <row r="102">
-      <c r="B102" s="17"/>
+      <c r="B102" s="18"/>
     </row>
     <row r="103">
-      <c r="B103" s="17"/>
+      <c r="B103" s="18"/>
     </row>
     <row r="104">
-      <c r="B104" s="17"/>
+      <c r="B104" s="18"/>
     </row>
     <row r="105">
-      <c r="B105" s="17"/>
+      <c r="B105" s="18"/>
     </row>
     <row r="106">
-      <c r="B106" s="17"/>
+      <c r="B106" s="18"/>
     </row>
     <row r="107">
-      <c r="B107" s="17"/>
+      <c r="B107" s="18"/>
     </row>
     <row r="108">
-      <c r="B108" s="17"/>
+      <c r="B108" s="18"/>
     </row>
     <row r="109">
-      <c r="B109" s="17"/>
+      <c r="B109" s="18"/>
     </row>
     <row r="110">
-      <c r="B110" s="17"/>
+      <c r="B110" s="18"/>
     </row>
     <row r="111">
-      <c r="B111" s="17"/>
+      <c r="B111" s="18"/>
     </row>
     <row r="112">
-      <c r="B112" s="17"/>
+      <c r="B112" s="18"/>
     </row>
     <row r="113">
-      <c r="B113" s="17"/>
+      <c r="B113" s="18"/>
     </row>
     <row r="114">
-      <c r="B114" s="17"/>
+      <c r="B114" s="18"/>
     </row>
     <row r="115">
-      <c r="B115" s="17"/>
+      <c r="B115" s="18"/>
     </row>
     <row r="116">
-      <c r="B116" s="17"/>
+      <c r="B116" s="18"/>
     </row>
     <row r="117">
-      <c r="B117" s="17"/>
+      <c r="B117" s="18"/>
     </row>
     <row r="118">
-      <c r="B118" s="17"/>
+      <c r="B118" s="18"/>
     </row>
     <row r="119">
-      <c r="B119" s="17"/>
+      <c r="B119" s="18"/>
     </row>
     <row r="120">
-      <c r="B120" s="17"/>
+      <c r="B120" s="18"/>
     </row>
     <row r="121">
-      <c r="B121" s="17"/>
+      <c r="B121" s="18"/>
     </row>
     <row r="122">
-      <c r="B122" s="17"/>
+      <c r="B122" s="18"/>
     </row>
     <row r="123">
-      <c r="B123" s="17"/>
+      <c r="B123" s="18"/>
     </row>
     <row r="124">
-      <c r="B124" s="17"/>
+      <c r="B124" s="18"/>
     </row>
     <row r="125">
-      <c r="B125" s="17"/>
+      <c r="B125" s="18"/>
     </row>
     <row r="126">
-      <c r="B126" s="17"/>
+      <c r="B126" s="18"/>
     </row>
     <row r="127">
-      <c r="B127" s="17"/>
+      <c r="B127" s="18"/>
     </row>
     <row r="128">
-      <c r="B128" s="17"/>
+      <c r="B128" s="18"/>
     </row>
     <row r="129">
-      <c r="B129" s="17"/>
+      <c r="B129" s="18"/>
     </row>
     <row r="130">
-      <c r="B130" s="17"/>
+      <c r="B130" s="18"/>
     </row>
     <row r="131">
-      <c r="B131" s="17"/>
+      <c r="B131" s="18"/>
     </row>
     <row r="132">
-      <c r="B132" s="17"/>
+      <c r="B132" s="18"/>
     </row>
     <row r="133">
-      <c r="B133" s="17"/>
+      <c r="B133" s="18"/>
     </row>
     <row r="134">
-      <c r="B134" s="17"/>
+      <c r="B134" s="18"/>
     </row>
     <row r="135">
-      <c r="B135" s="17"/>
+      <c r="B135" s="18"/>
     </row>
     <row r="136">
-      <c r="B136" s="17"/>
+      <c r="B136" s="18"/>
     </row>
     <row r="137">
-      <c r="B137" s="17"/>
+      <c r="B137" s="18"/>
     </row>
     <row r="138">
-      <c r="B138" s="17"/>
+      <c r="B138" s="18"/>
     </row>
     <row r="139">
-      <c r="B139" s="17"/>
+      <c r="B139" s="18"/>
     </row>
     <row r="140">
-      <c r="B140" s="17"/>
+      <c r="B140" s="18"/>
     </row>
     <row r="141">
-      <c r="B141" s="17"/>
+      <c r="B141" s="18"/>
     </row>
     <row r="142">
-      <c r="B142" s="17"/>
+      <c r="B142" s="18"/>
     </row>
     <row r="143">
-      <c r="B143" s="17"/>
+      <c r="B143" s="18"/>
     </row>
     <row r="144">
-      <c r="B144" s="17"/>
+      <c r="B144" s="18"/>
     </row>
     <row r="145">
-      <c r="B145" s="17"/>
+      <c r="B145" s="18"/>
     </row>
     <row r="146">
-      <c r="B146" s="17"/>
+      <c r="B146" s="18"/>
     </row>
     <row r="147">
-      <c r="B147" s="17"/>
+      <c r="B147" s="18"/>
     </row>
     <row r="148">
-      <c r="B148" s="17"/>
+      <c r="B148" s="18"/>
     </row>
     <row r="149">
-      <c r="B149" s="17"/>
+      <c r="B149" s="18"/>
     </row>
     <row r="150">
-      <c r="B150" s="17"/>
+      <c r="B150" s="18"/>
     </row>
     <row r="151">
-      <c r="B151" s="17"/>
+      <c r="B151" s="18"/>
     </row>
     <row r="152">
-      <c r="B152" s="17"/>
+      <c r="B152" s="18"/>
     </row>
     <row r="153">
-      <c r="B153" s="17"/>
+      <c r="B153" s="18"/>
     </row>
     <row r="154">
-      <c r="B154" s="17"/>
+      <c r="B154" s="18"/>
     </row>
     <row r="155">
-      <c r="B155" s="17"/>
+      <c r="B155" s="18"/>
     </row>
     <row r="156">
-      <c r="B156" s="17"/>
+      <c r="B156" s="18"/>
     </row>
     <row r="157">
-      <c r="B157" s="17"/>
+      <c r="B157" s="18"/>
     </row>
     <row r="158">
-      <c r="B158" s="17"/>
+      <c r="B158" s="18"/>
     </row>
     <row r="159">
-      <c r="B159" s="17"/>
+      <c r="B159" s="18"/>
     </row>
     <row r="160">
-      <c r="B160" s="17"/>
+      <c r="B160" s="18"/>
     </row>
     <row r="161">
-      <c r="B161" s="17"/>
+      <c r="B161" s="18"/>
     </row>
     <row r="162">
-      <c r="B162" s="17"/>
+      <c r="B162" s="18"/>
     </row>
     <row r="163">
-      <c r="B163" s="17"/>
+      <c r="B163" s="18"/>
     </row>
     <row r="164">
-      <c r="B164" s="17"/>
+      <c r="B164" s="18"/>
     </row>
     <row r="165">
-      <c r="B165" s="17"/>
+      <c r="B165" s="18"/>
     </row>
     <row r="166">
-      <c r="B166" s="17"/>
+      <c r="B166" s="18"/>
     </row>
     <row r="167">
-      <c r="B167" s="17"/>
+      <c r="B167" s="18"/>
     </row>
     <row r="168">
-      <c r="B168" s="17"/>
+      <c r="B168" s="18"/>
     </row>
     <row r="169">
-      <c r="B169" s="17"/>
+      <c r="B169" s="18"/>
     </row>
     <row r="170">
-      <c r="B170" s="17"/>
+      <c r="B170" s="18"/>
     </row>
     <row r="171">
-      <c r="B171" s="17"/>
+      <c r="B171" s="18"/>
     </row>
     <row r="172">
-      <c r="B172" s="17"/>
+      <c r="B172" s="18"/>
     </row>
     <row r="173">
-      <c r="B173" s="17"/>
+      <c r="B173" s="18"/>
     </row>
     <row r="174">
-      <c r="B174" s="17"/>
+      <c r="B174" s="18"/>
     </row>
     <row r="175">
-      <c r="B175" s="17"/>
+      <c r="B175" s="18"/>
     </row>
     <row r="176">
-      <c r="B176" s="17"/>
+      <c r="B176" s="18"/>
     </row>
     <row r="177">
-      <c r="B177" s="17"/>
+      <c r="B177" s="18"/>
     </row>
     <row r="178">
-      <c r="B178" s="17"/>
+      <c r="B178" s="18"/>
     </row>
     <row r="179">
-      <c r="B179" s="17"/>
+      <c r="B179" s="18"/>
     </row>
     <row r="180">
-      <c r="B180" s="17"/>
+      <c r="B180" s="18"/>
     </row>
     <row r="181">
-      <c r="B181" s="17"/>
+      <c r="B181" s="18"/>
     </row>
     <row r="182">
-      <c r="B182" s="17"/>
+      <c r="B182" s="18"/>
     </row>
     <row r="183">
-      <c r="B183" s="17"/>
+      <c r="B183" s="18"/>
     </row>
     <row r="184">
-      <c r="B184" s="17"/>
+      <c r="B184" s="18"/>
     </row>
     <row r="185">
-      <c r="B185" s="17"/>
+      <c r="B185" s="18"/>
     </row>
     <row r="186">
-      <c r="B186" s="17"/>
+      <c r="B186" s="18"/>
     </row>
     <row r="187">
-      <c r="B187" s="17"/>
+      <c r="B187" s="18"/>
     </row>
     <row r="188">
-      <c r="B188" s="17"/>
+      <c r="B188" s="18"/>
     </row>
     <row r="189">
-      <c r="B189" s="17"/>
+      <c r="B189" s="18"/>
     </row>
     <row r="190">
-      <c r="B190" s="17"/>
+      <c r="B190" s="18"/>
     </row>
     <row r="191">
-      <c r="B191" s="17"/>
+      <c r="B191" s="18"/>
     </row>
     <row r="192">
-      <c r="B192" s="17"/>
+      <c r="B192" s="18"/>
     </row>
     <row r="193">
-      <c r="B193" s="17"/>
+      <c r="B193" s="18"/>
     </row>
     <row r="194">
-      <c r="B194" s="17"/>
+      <c r="B194" s="18"/>
     </row>
     <row r="195">
-      <c r="B195" s="17"/>
+      <c r="B195" s="18"/>
     </row>
     <row r="196">
-      <c r="B196" s="17"/>
+      <c r="B196" s="18"/>
     </row>
     <row r="197">
-      <c r="B197" s="17"/>
+      <c r="B197" s="18"/>
     </row>
     <row r="198">
-      <c r="B198" s="17"/>
+      <c r="B198" s="18"/>
     </row>
     <row r="199">
-      <c r="B199" s="17"/>
+      <c r="B199" s="18"/>
     </row>
     <row r="200">
-      <c r="B200" s="17"/>
+      <c r="B200" s="18"/>
     </row>
     <row r="201">
-      <c r="B201" s="17"/>
+      <c r="B201" s="18"/>
     </row>
     <row r="202">
-      <c r="B202" s="17"/>
+      <c r="B202" s="18"/>
     </row>
     <row r="203">
-      <c r="B203" s="17"/>
+      <c r="B203" s="18"/>
     </row>
     <row r="204">
-      <c r="B204" s="17"/>
+      <c r="B204" s="18"/>
     </row>
     <row r="205">
-      <c r="B205" s="17"/>
+      <c r="B205" s="18"/>
     </row>
     <row r="206">
-      <c r="B206" s="17"/>
+      <c r="B206" s="18"/>
     </row>
     <row r="207">
-      <c r="B207" s="17"/>
+      <c r="B207" s="18"/>
     </row>
     <row r="208">
-      <c r="B208" s="17"/>
+      <c r="B208" s="18"/>
     </row>
     <row r="209">
-      <c r="B209" s="17"/>
+      <c r="B209" s="18"/>
     </row>
     <row r="210">
-      <c r="B210" s="17"/>
+      <c r="B210" s="18"/>
     </row>
     <row r="211">
-      <c r="B211" s="17"/>
+      <c r="B211" s="18"/>
     </row>
     <row r="212">
-      <c r="B212" s="17"/>
+      <c r="B212" s="18"/>
     </row>
     <row r="213">
-      <c r="B213" s="17"/>
+      <c r="B213" s="18"/>
     </row>
     <row r="214">
-      <c r="B214" s="17"/>
+      <c r="B214" s="18"/>
     </row>
     <row r="215">
-      <c r="B215" s="17"/>
+      <c r="B215" s="18"/>
     </row>
     <row r="216">
-      <c r="B216" s="17"/>
+      <c r="B216" s="18"/>
     </row>
     <row r="217">
-      <c r="B217" s="17"/>
+      <c r="B217" s="18"/>
     </row>
     <row r="218">
-      <c r="B218" s="17"/>
+      <c r="B218" s="18"/>
     </row>
     <row r="219">
-      <c r="B219" s="17"/>
+      <c r="B219" s="18"/>
     </row>
     <row r="220">
-      <c r="B220" s="17"/>
+      <c r="B220" s="18"/>
     </row>
     <row r="221">
-      <c r="B221" s="17"/>
+      <c r="B221" s="18"/>
     </row>
     <row r="222">
-      <c r="B222" s="17"/>
+      <c r="B222" s="18"/>
     </row>
     <row r="223">
-      <c r="B223" s="17"/>
+      <c r="B223" s="18"/>
     </row>
     <row r="224">
-      <c r="B224" s="17"/>
+      <c r="B224" s="18"/>
     </row>
     <row r="225">
-      <c r="B225" s="17"/>
+      <c r="B225" s="18"/>
     </row>
     <row r="226">
-      <c r="B226" s="17"/>
+      <c r="B226" s="18"/>
     </row>
     <row r="227">
-      <c r="B227" s="17"/>
+      <c r="B227" s="18"/>
     </row>
     <row r="228">
-      <c r="B228" s="17"/>
+      <c r="B228" s="18"/>
     </row>
     <row r="229">
-      <c r="B229" s="17"/>
+      <c r="B229" s="18"/>
     </row>
     <row r="230">
-      <c r="B230" s="17"/>
+      <c r="B230" s="18"/>
     </row>
     <row r="231">
-      <c r="B231" s="17"/>
+      <c r="B231" s="18"/>
     </row>
     <row r="232">
-      <c r="B232" s="17"/>
+      <c r="B232" s="18"/>
     </row>
     <row r="233">
-      <c r="B233" s="17"/>
+      <c r="B233" s="18"/>
     </row>
     <row r="234">
-      <c r="B234" s="17"/>
+      <c r="B234" s="18"/>
     </row>
     <row r="235">
-      <c r="B235" s="17"/>
+      <c r="B235" s="18"/>
     </row>
     <row r="236">
-      <c r="B236" s="17"/>
+      <c r="B236" s="18"/>
     </row>
     <row r="237">
-      <c r="B237" s="17"/>
+      <c r="B237" s="18"/>
     </row>
     <row r="238">
-      <c r="B238" s="17"/>
+      <c r="B238" s="18"/>
     </row>
     <row r="239">
-      <c r="B239" s="17"/>
+      <c r="B239" s="18"/>
     </row>
     <row r="240">
-      <c r="B240" s="17"/>
+      <c r="B240" s="18"/>
     </row>
     <row r="241">
-      <c r="B241" s="17"/>
+      <c r="B241" s="18"/>
     </row>
     <row r="242">
-      <c r="B242" s="17"/>
+      <c r="B242" s="18"/>
     </row>
     <row r="243">
-      <c r="B243" s="17"/>
+      <c r="B243" s="18"/>
     </row>
     <row r="244">
-      <c r="B244" s="17"/>
+      <c r="B244" s="18"/>
     </row>
     <row r="245">
-      <c r="B245" s="17"/>
+      <c r="B245" s="18"/>
     </row>
     <row r="246">
-      <c r="B246" s="17"/>
+      <c r="B246" s="18"/>
     </row>
     <row r="247">
-      <c r="B247" s="17"/>
+      <c r="B247" s="18"/>
     </row>
     <row r="248">
-      <c r="B248" s="17"/>
+      <c r="B248" s="18"/>
     </row>
     <row r="249">
-      <c r="B249" s="17"/>
+      <c r="B249" s="18"/>
     </row>
     <row r="250">
-      <c r="B250" s="17"/>
+      <c r="B250" s="18"/>
     </row>
     <row r="251">
-      <c r="B251" s="17"/>
+      <c r="B251" s="18"/>
     </row>
     <row r="252">
-      <c r="B252" s="17"/>
+      <c r="B252" s="18"/>
     </row>
     <row r="253">
-      <c r="B253" s="17"/>
+      <c r="B253" s="18"/>
     </row>
     <row r="254">
-      <c r="B254" s="17"/>
+      <c r="B254" s="18"/>
     </row>
     <row r="255">
-      <c r="B255" s="17"/>
+      <c r="B255" s="18"/>
     </row>
     <row r="256">
-      <c r="B256" s="17"/>
+      <c r="B256" s="18"/>
     </row>
     <row r="257">
-      <c r="B257" s="17"/>
+      <c r="B257" s="18"/>
     </row>
     <row r="258">
-      <c r="B258" s="17"/>
+      <c r="B258" s="18"/>
     </row>
     <row r="259">
-      <c r="B259" s="17"/>
+      <c r="B259" s="18"/>
     </row>
     <row r="260">
-      <c r="B260" s="17"/>
+      <c r="B260" s="18"/>
     </row>
     <row r="261">
-      <c r="B261" s="17"/>
+      <c r="B261" s="18"/>
     </row>
     <row r="262">
-      <c r="B262" s="17"/>
+      <c r="B262" s="18"/>
     </row>
     <row r="263">
-      <c r="B263" s="17"/>
+      <c r="B263" s="18"/>
     </row>
     <row r="264">
-      <c r="B264" s="17"/>
+      <c r="B264" s="18"/>
     </row>
     <row r="265">
-      <c r="B265" s="17"/>
+      <c r="B265" s="18"/>
     </row>
     <row r="266">
-      <c r="B266" s="17"/>
+      <c r="B266" s="18"/>
     </row>
     <row r="267">
-      <c r="B267" s="17"/>
+      <c r="B267" s="18"/>
     </row>
     <row r="268">
-      <c r="B268" s="17"/>
+      <c r="B268" s="18"/>
     </row>
     <row r="269">
-      <c r="B269" s="17"/>
+      <c r="B269" s="18"/>
     </row>
     <row r="270">
-      <c r="B270" s="17"/>
+      <c r="B270" s="18"/>
     </row>
     <row r="271">
-      <c r="B271" s="17"/>
+      <c r="B271" s="18"/>
     </row>
     <row r="272">
-      <c r="B272" s="17"/>
+      <c r="B272" s="18"/>
     </row>
     <row r="273">
-      <c r="B273" s="17"/>
+      <c r="B273" s="18"/>
     </row>
     <row r="274">
-      <c r="B274" s="17"/>
+      <c r="B274" s="18"/>
     </row>
     <row r="275">
-      <c r="B275" s="17"/>
+      <c r="B275" s="18"/>
     </row>
     <row r="276">
-      <c r="B276" s="17"/>
+      <c r="B276" s="18"/>
     </row>
     <row r="277">
-      <c r="B277" s="17"/>
+      <c r="B277" s="18"/>
     </row>
     <row r="278">
-      <c r="B278" s="17"/>
+      <c r="B278" s="18"/>
     </row>
     <row r="279">
-      <c r="B279" s="17"/>
+      <c r="B279" s="18"/>
     </row>
     <row r="280">
-      <c r="B280" s="17"/>
+      <c r="B280" s="18"/>
     </row>
     <row r="281">
-      <c r="B281" s="17"/>
+      <c r="B281" s="18"/>
     </row>
     <row r="282">
-      <c r="B282" s="17"/>
+      <c r="B282" s="18"/>
     </row>
     <row r="283">
-      <c r="B283" s="17"/>
+      <c r="B283" s="18"/>
     </row>
     <row r="284">
-      <c r="B284" s="17"/>
+      <c r="B284" s="18"/>
     </row>
     <row r="285">
-      <c r="B285" s="17"/>
+      <c r="B285" s="18"/>
     </row>
     <row r="286">
-      <c r="B286" s="17"/>
+      <c r="B286" s="18"/>
     </row>
     <row r="287">
-      <c r="B287" s="17"/>
+      <c r="B287" s="18"/>
     </row>
     <row r="288">
-      <c r="B288" s="17"/>
+      <c r="B288" s="18"/>
     </row>
     <row r="289">
-      <c r="B289" s="17"/>
+      <c r="B289" s="18"/>
     </row>
     <row r="290">
-      <c r="B290" s="17"/>
+      <c r="B290" s="18"/>
     </row>
     <row r="291">
-      <c r="B291" s="17"/>
+      <c r="B291" s="18"/>
     </row>
     <row r="292">
-      <c r="B292" s="17"/>
+      <c r="B292" s="18"/>
     </row>
     <row r="293">
-      <c r="B293" s="17"/>
+      <c r="B293" s="18"/>
     </row>
     <row r="294">
-      <c r="B294" s="17"/>
+      <c r="B294" s="18"/>
     </row>
     <row r="295">
-      <c r="B295" s="17"/>
+      <c r="B295" s="18"/>
     </row>
     <row r="296">
-      <c r="B296" s="17"/>
+      <c r="B296" s="18"/>
     </row>
     <row r="297">
-      <c r="B297" s="17"/>
+      <c r="B297" s="18"/>
     </row>
     <row r="298">
-      <c r="B298" s="17"/>
+      <c r="B298" s="18"/>
     </row>
     <row r="299">
-      <c r="B299" s="17"/>
+      <c r="B299" s="18"/>
     </row>
     <row r="300">
-      <c r="B300" s="17"/>
+      <c r="B300" s="18"/>
     </row>
     <row r="301">
-      <c r="B301" s="17"/>
+      <c r="B301" s="18"/>
     </row>
     <row r="302">
-      <c r="B302" s="17"/>
+      <c r="B302" s="18"/>
     </row>
     <row r="303">
-      <c r="B303" s="17"/>
+      <c r="B303" s="18"/>
     </row>
     <row r="304">
-      <c r="B304" s="17"/>
+      <c r="B304" s="18"/>
     </row>
     <row r="305">
-      <c r="B305" s="17"/>
+      <c r="B305" s="18"/>
     </row>
     <row r="306">
-      <c r="B306" s="17"/>
+      <c r="B306" s="18"/>
     </row>
     <row r="307">
-      <c r="B307" s="17"/>
+      <c r="B307" s="18"/>
     </row>
     <row r="308">
-      <c r="B308" s="17"/>
+      <c r="B308" s="18"/>
     </row>
     <row r="309">
-      <c r="B309" s="17"/>
+      <c r="B309" s="18"/>
     </row>
     <row r="310">
-      <c r="B310" s="17"/>
+      <c r="B310" s="18"/>
     </row>
     <row r="311">
-      <c r="B311" s="17"/>
+      <c r="B311" s="18"/>
     </row>
     <row r="312">
-      <c r="B312" s="17"/>
+      <c r="B312" s="18"/>
     </row>
     <row r="313">
-      <c r="B313" s="17"/>
+      <c r="B313" s="18"/>
     </row>
     <row r="314">
-      <c r="B314" s="17"/>
+      <c r="B314" s="18"/>
     </row>
     <row r="315">
-      <c r="B315" s="17"/>
+      <c r="B315" s="18"/>
     </row>
     <row r="316">
-      <c r="B316" s="17"/>
+      <c r="B316" s="18"/>
     </row>
     <row r="317">
-      <c r="B317" s="17"/>
+      <c r="B317" s="18"/>
     </row>
     <row r="318">
-      <c r="B318" s="17"/>
+      <c r="B318" s="18"/>
     </row>
     <row r="319">
-      <c r="B319" s="17"/>
+      <c r="B319" s="18"/>
     </row>
     <row r="320">
-      <c r="B320" s="17"/>
+      <c r="B320" s="18"/>
     </row>
     <row r="321">
-      <c r="B321" s="17"/>
+      <c r="B321" s="18"/>
     </row>
     <row r="322">
-      <c r="B322" s="17"/>
+      <c r="B322" s="18"/>
     </row>
     <row r="323">
-      <c r="B323" s="17"/>
+      <c r="B323" s="18"/>
     </row>
     <row r="324">
-      <c r="B324" s="17"/>
+      <c r="B324" s="18"/>
     </row>
     <row r="325">
-      <c r="B325" s="17"/>
+      <c r="B325" s="18"/>
     </row>
     <row r="326">
-      <c r="B326" s="17"/>
+      <c r="B326" s="18"/>
     </row>
     <row r="327">
-      <c r="B327" s="17"/>
+      <c r="B327" s="18"/>
     </row>
     <row r="328">
-      <c r="B328" s="17"/>
+      <c r="B328" s="18"/>
     </row>
     <row r="329">
-      <c r="B329" s="17"/>
+      <c r="B329" s="18"/>
     </row>
     <row r="330">
-      <c r="B330" s="17"/>
+      <c r="B330" s="18"/>
     </row>
     <row r="331">
-      <c r="B331" s="17"/>
+      <c r="B331" s="18"/>
     </row>
     <row r="332">
-      <c r="B332" s="17"/>
+      <c r="B332" s="18"/>
     </row>
     <row r="333">
-      <c r="B333" s="17"/>
+      <c r="B333" s="18"/>
     </row>
     <row r="334">
-      <c r="B334" s="17"/>
+      <c r="B334" s="18"/>
     </row>
     <row r="335">
-      <c r="B335" s="17"/>
+      <c r="B335" s="18"/>
     </row>
     <row r="336">
-      <c r="B336" s="17"/>
+      <c r="B336" s="18"/>
     </row>
     <row r="337">
-      <c r="B337" s="17"/>
+      <c r="B337" s="18"/>
     </row>
     <row r="338">
-      <c r="B338" s="17"/>
+      <c r="B338" s="18"/>
     </row>
     <row r="339">
-      <c r="B339" s="17"/>
+      <c r="B339" s="18"/>
     </row>
     <row r="340">
-      <c r="B340" s="17"/>
+      <c r="B340" s="18"/>
     </row>
     <row r="341">
-      <c r="B341" s="17"/>
+      <c r="B341" s="18"/>
     </row>
     <row r="342">
-      <c r="B342" s="17"/>
+      <c r="B342" s="18"/>
     </row>
     <row r="343">
-      <c r="B343" s="17"/>
+      <c r="B343" s="18"/>
     </row>
     <row r="344">
-      <c r="B344" s="17"/>
+      <c r="B344" s="18"/>
     </row>
     <row r="345">
-      <c r="B345" s="17"/>
+      <c r="B345" s="18"/>
     </row>
     <row r="346">
-      <c r="B346" s="17"/>
+      <c r="B346" s="18"/>
     </row>
     <row r="347">
-      <c r="B347" s="17"/>
+      <c r="B347" s="18"/>
     </row>
     <row r="348">
-      <c r="B348" s="17"/>
+      <c r="B348" s="18"/>
     </row>
     <row r="349">
-      <c r="B349" s="17"/>
+      <c r="B349" s="18"/>
     </row>
     <row r="350">
-      <c r="B350" s="17"/>
+      <c r="B350" s="18"/>
     </row>
     <row r="351">
-      <c r="B351" s="17"/>
+      <c r="B351" s="18"/>
     </row>
     <row r="352">
-      <c r="B352" s="17"/>
+      <c r="B352" s="18"/>
     </row>
     <row r="353">
-      <c r="B353" s="17"/>
+      <c r="B353" s="18"/>
     </row>
     <row r="354">
-      <c r="B354" s="17"/>
+      <c r="B354" s="18"/>
     </row>
     <row r="355">
-      <c r="B355" s="17"/>
+      <c r="B355" s="18"/>
     </row>
     <row r="356">
-      <c r="B356" s="17"/>
+      <c r="B356" s="18"/>
     </row>
     <row r="357">
-      <c r="B357" s="17"/>
+      <c r="B357" s="18"/>
     </row>
     <row r="358">
-      <c r="B358" s="17"/>
+      <c r="B358" s="18"/>
     </row>
     <row r="359">
-      <c r="B359" s="17"/>
+      <c r="B359" s="18"/>
     </row>
     <row r="360">
-      <c r="B360" s="17"/>
+      <c r="B360" s="18"/>
     </row>
     <row r="361">
-      <c r="B361" s="17"/>
+      <c r="B361" s="18"/>
     </row>
     <row r="362">
-      <c r="B362" s="17"/>
+      <c r="B362" s="18"/>
     </row>
     <row r="363">
-      <c r="B363" s="17"/>
+      <c r="B363" s="18"/>
     </row>
     <row r="364">
-      <c r="B364" s="17"/>
+      <c r="B364" s="18"/>
     </row>
     <row r="365">
-      <c r="B365" s="17"/>
+      <c r="B365" s="18"/>
     </row>
     <row r="366">
-      <c r="B366" s="17"/>
+      <c r="B366" s="18"/>
     </row>
     <row r="367">
-      <c r="B367" s="17"/>
+      <c r="B367" s="18"/>
     </row>
     <row r="368">
-      <c r="B368" s="17"/>
+      <c r="B368" s="18"/>
     </row>
     <row r="369">
-      <c r="B369" s="17"/>
+      <c r="B369" s="18"/>
     </row>
     <row r="370">
-      <c r="B370" s="17"/>
+      <c r="B370" s="18"/>
     </row>
     <row r="371">
-      <c r="B371" s="17"/>
+      <c r="B371" s="18"/>
     </row>
     <row r="372">
-      <c r="B372" s="17"/>
+      <c r="B372" s="18"/>
     </row>
     <row r="373">
-      <c r="B373" s="17"/>
+      <c r="B373" s="18"/>
     </row>
     <row r="374">
-      <c r="B374" s="17"/>
+      <c r="B374" s="18"/>
     </row>
     <row r="375">
-      <c r="B375" s="17"/>
+      <c r="B375" s="18"/>
     </row>
     <row r="376">
-      <c r="B376" s="17"/>
+      <c r="B376" s="18"/>
     </row>
     <row r="377">
-      <c r="B377" s="17"/>
+      <c r="B377" s="18"/>
     </row>
     <row r="378">
-      <c r="B378" s="17"/>
+      <c r="B378" s="18"/>
     </row>
     <row r="379">
-      <c r="B379" s="17"/>
+      <c r="B379" s="18"/>
     </row>
     <row r="380">
-      <c r="B380" s="17"/>
+      <c r="B380" s="18"/>
     </row>
     <row r="381">
-      <c r="B381" s="17"/>
+      <c r="B381" s="18"/>
     </row>
     <row r="382">
-      <c r="B382" s="17"/>
+      <c r="B382" s="18"/>
     </row>
     <row r="383">
-      <c r="B383" s="17"/>
+      <c r="B383" s="18"/>
     </row>
     <row r="384">
-      <c r="B384" s="17"/>
+      <c r="B384" s="18"/>
     </row>
     <row r="385">
-      <c r="B385" s="17"/>
+      <c r="B385" s="18"/>
     </row>
     <row r="386">
-      <c r="B386" s="17"/>
+      <c r="B386" s="18"/>
     </row>
     <row r="387">
-      <c r="B387" s="17"/>
+      <c r="B387" s="18"/>
     </row>
     <row r="388">
-      <c r="B388" s="17"/>
+      <c r="B388" s="18"/>
     </row>
     <row r="389">
-      <c r="B389" s="17"/>
+      <c r="B389" s="18"/>
     </row>
     <row r="390">
-      <c r="B390" s="17"/>
+      <c r="B390" s="18"/>
     </row>
     <row r="391">
-      <c r="B391" s="17"/>
+      <c r="B391" s="18"/>
     </row>
     <row r="392">
-      <c r="B392" s="17"/>
+      <c r="B392" s="18"/>
     </row>
     <row r="393">
-      <c r="B393" s="17"/>
+      <c r="B393" s="18"/>
     </row>
     <row r="394">
-      <c r="B394" s="17"/>
+      <c r="B394" s="18"/>
     </row>
     <row r="395">
-      <c r="B395" s="17"/>
+      <c r="B395" s="18"/>
     </row>
     <row r="396">
-      <c r="B396" s="17"/>
+      <c r="B396" s="18"/>
     </row>
     <row r="397">
-      <c r="B397" s="17"/>
+      <c r="B397" s="18"/>
     </row>
     <row r="398">
-      <c r="B398" s="17"/>
+      <c r="B398" s="18"/>
     </row>
     <row r="399">
-      <c r="B399" s="17"/>
+      <c r="B399" s="18"/>
     </row>
     <row r="400">
-      <c r="B400" s="17"/>
+      <c r="B400" s="18"/>
     </row>
     <row r="401">
-      <c r="B401" s="17"/>
+      <c r="B401" s="18"/>
     </row>
     <row r="402">
-      <c r="B402" s="17"/>
+      <c r="B402" s="18"/>
     </row>
     <row r="403">
-      <c r="B403" s="17"/>
+      <c r="B403" s="18"/>
     </row>
     <row r="404">
-      <c r="B404" s="17"/>
+      <c r="B404" s="18"/>
     </row>
     <row r="405">
-      <c r="B405" s="17"/>
+      <c r="B405" s="18"/>
     </row>
     <row r="406">
-      <c r="B406" s="17"/>
+      <c r="B406" s="18"/>
     </row>
     <row r="407">
-      <c r="B407" s="17"/>
+      <c r="B407" s="18"/>
     </row>
     <row r="408">
-      <c r="B408" s="17"/>
+      <c r="B408" s="18"/>
     </row>
     <row r="409">
-      <c r="B409" s="17"/>
+      <c r="B409" s="18"/>
     </row>
     <row r="410">
-      <c r="B410" s="17"/>
+      <c r="B410" s="18"/>
     </row>
     <row r="411">
-      <c r="B411" s="17"/>
+      <c r="B411" s="18"/>
     </row>
     <row r="412">
-      <c r="B412" s="17"/>
+      <c r="B412" s="18"/>
     </row>
     <row r="413">
-      <c r="B413" s="17"/>
+      <c r="B413" s="18"/>
     </row>
     <row r="414">
-      <c r="B414" s="17"/>
+      <c r="B414" s="18"/>
     </row>
     <row r="415">
-      <c r="B415" s="17"/>
+      <c r="B415" s="18"/>
     </row>
     <row r="416">
-      <c r="B416" s="17"/>
+      <c r="B416" s="18"/>
     </row>
     <row r="417">
-      <c r="B417" s="17"/>
+      <c r="B417" s="18"/>
     </row>
     <row r="418">
-      <c r="B418" s="17"/>
+      <c r="B418" s="18"/>
     </row>
     <row r="419">
-      <c r="B419" s="17"/>
+      <c r="B419" s="18"/>
     </row>
     <row r="420">
-      <c r="B420" s="17"/>
+      <c r="B420" s="18"/>
     </row>
     <row r="421">
-      <c r="B421" s="17"/>
+      <c r="B421" s="18"/>
     </row>
     <row r="422">
-      <c r="B422" s="17"/>
+      <c r="B422" s="18"/>
     </row>
     <row r="423">
-      <c r="B423" s="17"/>
+      <c r="B423" s="18"/>
     </row>
     <row r="424">
-      <c r="B424" s="17"/>
+      <c r="B424" s="18"/>
     </row>
     <row r="425">
-      <c r="B425" s="17"/>
+      <c r="B425" s="18"/>
     </row>
     <row r="426">
-      <c r="B426" s="17"/>
+      <c r="B426" s="18"/>
     </row>
     <row r="427">
-      <c r="B427" s="17"/>
+      <c r="B427" s="18"/>
     </row>
     <row r="428">
-      <c r="B428" s="17"/>
+      <c r="B428" s="18"/>
     </row>
     <row r="429">
-      <c r="B429" s="17"/>
+      <c r="B429" s="18"/>
     </row>
     <row r="430">
-      <c r="B430" s="17"/>
+      <c r="B430" s="18"/>
     </row>
     <row r="431">
-      <c r="B431" s="17"/>
+      <c r="B431" s="18"/>
     </row>
     <row r="432">
-      <c r="B432" s="17"/>
+      <c r="B432" s="18"/>
     </row>
     <row r="433">
-      <c r="B433" s="17"/>
+      <c r="B433" s="18"/>
     </row>
     <row r="434">
-      <c r="B434" s="17"/>
+      <c r="B434" s="18"/>
     </row>
     <row r="435">
-      <c r="B435" s="17"/>
+      <c r="B435" s="18"/>
     </row>
     <row r="436">
-      <c r="B436" s="17"/>
+      <c r="B436" s="18"/>
     </row>
     <row r="437">
-      <c r="B437" s="17"/>
+      <c r="B437" s="18"/>
     </row>
     <row r="438">
-      <c r="B438" s="17"/>
+      <c r="B438" s="18"/>
     </row>
     <row r="439">
-      <c r="B439" s="17"/>
+      <c r="B439" s="18"/>
     </row>
     <row r="440">
-      <c r="B440" s="17"/>
+      <c r="B440" s="18"/>
     </row>
     <row r="441">
-      <c r="B441" s="17"/>
+      <c r="B441" s="18"/>
     </row>
     <row r="442">
-      <c r="B442" s="17"/>
+      <c r="B442" s="18"/>
     </row>
     <row r="443">
-      <c r="B443" s="17"/>
+      <c r="B443" s="18"/>
     </row>
     <row r="444">
-      <c r="B444" s="17"/>
+      <c r="B444" s="18"/>
     </row>
     <row r="445">
-      <c r="B445" s="17"/>
+      <c r="B445" s="18"/>
     </row>
     <row r="446">
-      <c r="B446" s="17"/>
+      <c r="B446" s="18"/>
     </row>
     <row r="447">
-      <c r="B447" s="17"/>
+      <c r="B447" s="18"/>
     </row>
     <row r="448">
-      <c r="B448" s="17"/>
+      <c r="B448" s="18"/>
     </row>
     <row r="449">
-      <c r="B449" s="17"/>
+      <c r="B449" s="18"/>
     </row>
     <row r="450">
-      <c r="B450" s="17"/>
+      <c r="B450" s="18"/>
     </row>
     <row r="451">
-      <c r="B451" s="17"/>
+      <c r="B451" s="18"/>
     </row>
     <row r="452">
-      <c r="B452" s="17"/>
+      <c r="B452" s="18"/>
     </row>
     <row r="453">
-      <c r="B453" s="17"/>
+      <c r="B453" s="18"/>
     </row>
     <row r="454">
-      <c r="B454" s="17"/>
+      <c r="B454" s="18"/>
     </row>
     <row r="455">
-      <c r="B455" s="17"/>
+      <c r="B455" s="18"/>
     </row>
     <row r="456">
-      <c r="B456" s="17"/>
+      <c r="B456" s="18"/>
     </row>
     <row r="457">
-      <c r="B457" s="17"/>
+      <c r="B457" s="18"/>
     </row>
     <row r="458">
-      <c r="B458" s="17"/>
+      <c r="B458" s="18"/>
     </row>
     <row r="459">
-      <c r="B459" s="17"/>
+      <c r="B459" s="18"/>
     </row>
     <row r="460">
-      <c r="B460" s="17"/>
+      <c r="B460" s="18"/>
     </row>
     <row r="461">
-      <c r="B461" s="17"/>
+      <c r="B461" s="18"/>
     </row>
     <row r="462">
-      <c r="B462" s="17"/>
+      <c r="B462" s="18"/>
     </row>
     <row r="463">
-      <c r="B463" s="17"/>
+      <c r="B463" s="18"/>
     </row>
     <row r="464">
-      <c r="B464" s="17"/>
+      <c r="B464" s="18"/>
     </row>
     <row r="465">
-      <c r="B465" s="17"/>
+      <c r="B465" s="18"/>
     </row>
     <row r="466">
-      <c r="B466" s="17"/>
+      <c r="B466" s="18"/>
     </row>
     <row r="467">
-      <c r="B467" s="17"/>
+      <c r="B467" s="18"/>
     </row>
     <row r="468">
-      <c r="B468" s="17"/>
+      <c r="B468" s="18"/>
     </row>
     <row r="469">
-      <c r="B469" s="17"/>
+      <c r="B469" s="18"/>
     </row>
     <row r="470">
-      <c r="B470" s="17"/>
+      <c r="B470" s="18"/>
     </row>
     <row r="471">
-      <c r="B471" s="17"/>
+      <c r="B471" s="18"/>
     </row>
     <row r="472">
-      <c r="B472" s="17"/>
+      <c r="B472" s="18"/>
     </row>
     <row r="473">
-      <c r="B473" s="17"/>
+      <c r="B473" s="18"/>
     </row>
     <row r="474">
-      <c r="B474" s="17"/>
+      <c r="B474" s="18"/>
     </row>
     <row r="475">
-      <c r="B475" s="17"/>
+      <c r="B475" s="18"/>
     </row>
     <row r="476">
-      <c r="B476" s="17"/>
+      <c r="B476" s="18"/>
     </row>
     <row r="477">
-      <c r="B477" s="17"/>
+      <c r="B477" s="18"/>
     </row>
     <row r="478">
-      <c r="B478" s="17"/>
+      <c r="B478" s="18"/>
     </row>
     <row r="479">
-      <c r="B479" s="17"/>
+      <c r="B479" s="18"/>
     </row>
     <row r="480">
-      <c r="B480" s="17"/>
+      <c r="B480" s="18"/>
     </row>
     <row r="481">
-      <c r="B481" s="17"/>
+      <c r="B481" s="18"/>
     </row>
     <row r="482">
-      <c r="B482" s="17"/>
+      <c r="B482" s="18"/>
     </row>
     <row r="483">
-      <c r="B483" s="17"/>
+      <c r="B483" s="18"/>
     </row>
     <row r="484">
-      <c r="B484" s="17"/>
+      <c r="B484" s="18"/>
     </row>
     <row r="485">
-      <c r="B485" s="17"/>
+      <c r="B485" s="18"/>
     </row>
     <row r="486">
-      <c r="B486" s="17"/>
+      <c r="B486" s="18"/>
     </row>
     <row r="487">
-      <c r="B487" s="17"/>
+      <c r="B487" s="18"/>
     </row>
     <row r="488">
-      <c r="B488" s="17"/>
+      <c r="B488" s="18"/>
     </row>
     <row r="489">
-      <c r="B489" s="17"/>
+      <c r="B489" s="18"/>
     </row>
     <row r="490">
-      <c r="B490" s="17"/>
+      <c r="B490" s="18"/>
     </row>
     <row r="491">
-      <c r="B491" s="17"/>
+      <c r="B491" s="18"/>
     </row>
     <row r="492">
-      <c r="B492" s="17"/>
+      <c r="B492" s="18"/>
     </row>
     <row r="493">
-      <c r="B493" s="17"/>
+      <c r="B493" s="18"/>
     </row>
     <row r="494">
-      <c r="B494" s="17"/>
+      <c r="B494" s="18"/>
     </row>
     <row r="495">
-      <c r="B495" s="17"/>
+      <c r="B495" s="18"/>
     </row>
     <row r="496">
-      <c r="B496" s="17"/>
+      <c r="B496" s="18"/>
     </row>
     <row r="497">
-      <c r="B497" s="17"/>
+      <c r="B497" s="18"/>
     </row>
     <row r="498">
-      <c r="B498" s="17"/>
+      <c r="B498" s="18"/>
     </row>
     <row r="499">
-      <c r="B499" s="17"/>
+      <c r="B499" s="18"/>
     </row>
     <row r="500">
-      <c r="B500" s="17"/>
+      <c r="B500" s="18"/>
     </row>
     <row r="501">
-      <c r="B501" s="17"/>
+      <c r="B501" s="18"/>
     </row>
     <row r="502">
-      <c r="B502" s="17"/>
+      <c r="B502" s="18"/>
     </row>
     <row r="503">
-      <c r="B503" s="17"/>
+      <c r="B503" s="18"/>
     </row>
     <row r="504">
-      <c r="B504" s="17"/>
+      <c r="B504" s="18"/>
     </row>
     <row r="505">
-      <c r="B505" s="17"/>
+      <c r="B505" s="18"/>
     </row>
     <row r="506">
-      <c r="B506" s="17"/>
+      <c r="B506" s="18"/>
     </row>
     <row r="507">
-      <c r="B507" s="17"/>
+      <c r="B507" s="18"/>
     </row>
     <row r="508">
-      <c r="B508" s="17"/>
+      <c r="B508" s="18"/>
     </row>
     <row r="509">
-      <c r="B509" s="17"/>
+      <c r="B509" s="18"/>
     </row>
     <row r="510">
-      <c r="B510" s="17"/>
+      <c r="B510" s="18"/>
     </row>
     <row r="511">
-      <c r="B511" s="17"/>
+      <c r="B511" s="18"/>
     </row>
     <row r="512">
-      <c r="B512" s="17"/>
+      <c r="B512" s="18"/>
     </row>
     <row r="513">
-      <c r="B513" s="17"/>
+      <c r="B513" s="18"/>
     </row>
     <row r="514">
-      <c r="B514" s="17"/>
+      <c r="B514" s="18"/>
     </row>
     <row r="515">
-      <c r="B515" s="17"/>
+      <c r="B515" s="18"/>
     </row>
     <row r="516">
-      <c r="B516" s="17"/>
+      <c r="B516" s="18"/>
     </row>
     <row r="517">
-      <c r="B517" s="17"/>
+      <c r="B517" s="18"/>
     </row>
     <row r="518">
-      <c r="B518" s="17"/>
+      <c r="B518" s="18"/>
     </row>
     <row r="519">
-      <c r="B519" s="17"/>
+      <c r="B519" s="18"/>
     </row>
     <row r="520">
-      <c r="B520" s="17"/>
+      <c r="B520" s="18"/>
     </row>
     <row r="521">
-      <c r="B521" s="17"/>
+      <c r="B521" s="18"/>
     </row>
     <row r="522">
-      <c r="B522" s="17"/>
+      <c r="B522" s="18"/>
     </row>
     <row r="523">
-      <c r="B523" s="17"/>
+      <c r="B523" s="18"/>
     </row>
     <row r="524">
-      <c r="B524" s="17"/>
+      <c r="B524" s="18"/>
     </row>
     <row r="525">
-      <c r="B525" s="17"/>
+      <c r="B525" s="18"/>
     </row>
     <row r="526">
-      <c r="B526" s="17"/>
+      <c r="B526" s="18"/>
     </row>
     <row r="527">
-      <c r="B527" s="17"/>
+      <c r="B527" s="18"/>
     </row>
     <row r="528">
-      <c r="B528" s="17"/>
+      <c r="B528" s="18"/>
     </row>
     <row r="529">
-      <c r="B529" s="17"/>
+      <c r="B529" s="18"/>
     </row>
     <row r="530">
-      <c r="B530" s="17"/>
+      <c r="B530" s="18"/>
     </row>
     <row r="531">
-      <c r="B531" s="17"/>
+      <c r="B531" s="18"/>
     </row>
     <row r="532">
-      <c r="B532" s="17"/>
+      <c r="B532" s="18"/>
     </row>
     <row r="533">
-      <c r="B533" s="17"/>
+      <c r="B533" s="18"/>
     </row>
     <row r="534">
-      <c r="B534" s="17"/>
+      <c r="B534" s="18"/>
     </row>
     <row r="535">
-      <c r="B535" s="17"/>
+      <c r="B535" s="18"/>
     </row>
     <row r="536">
-      <c r="B536" s="17"/>
+      <c r="B536" s="18"/>
     </row>
     <row r="537">
-      <c r="B537" s="17"/>
+      <c r="B537" s="18"/>
     </row>
     <row r="538">
-      <c r="B538" s="17"/>
+      <c r="B538" s="18"/>
     </row>
     <row r="539">
-      <c r="B539" s="17"/>
+      <c r="B539" s="18"/>
     </row>
     <row r="540">
-      <c r="B540" s="17"/>
+      <c r="B540" s="18"/>
     </row>
     <row r="541">
-      <c r="B541" s="17"/>
+      <c r="B541" s="18"/>
     </row>
     <row r="542">
-      <c r="B542" s="17"/>
+      <c r="B542" s="18"/>
     </row>
     <row r="543">
-      <c r="B543" s="17"/>
+      <c r="B543" s="18"/>
     </row>
     <row r="544">
-      <c r="B544" s="17"/>
+      <c r="B544" s="18"/>
     </row>
     <row r="545">
-      <c r="B545" s="17"/>
+      <c r="B545" s="18"/>
     </row>
     <row r="546">
-      <c r="B546" s="17"/>
+      <c r="B546" s="18"/>
     </row>
     <row r="547">
-      <c r="B547" s="17"/>
+      <c r="B547" s="18"/>
     </row>
     <row r="548">
-      <c r="B548" s="17"/>
+      <c r="B548" s="18"/>
     </row>
     <row r="549">
-      <c r="B549" s="17"/>
+      <c r="B549" s="18"/>
     </row>
     <row r="550">
-      <c r="B550" s="17"/>
+      <c r="B550" s="18"/>
     </row>
     <row r="551">
-      <c r="B551" s="17"/>
+      <c r="B551" s="18"/>
     </row>
     <row r="552">
-      <c r="B552" s="17"/>
+      <c r="B552" s="18"/>
     </row>
     <row r="553">
-      <c r="B553" s="17"/>
+      <c r="B553" s="18"/>
     </row>
     <row r="554">
-      <c r="B554" s="17"/>
+      <c r="B554" s="18"/>
     </row>
     <row r="555">
-      <c r="B555" s="17"/>
+      <c r="B555" s="18"/>
     </row>
     <row r="556">
-      <c r="B556" s="17"/>
+      <c r="B556" s="18"/>
     </row>
     <row r="557">
-      <c r="B557" s="17"/>
+      <c r="B557" s="18"/>
     </row>
     <row r="558">
-      <c r="B558" s="17"/>
+      <c r="B558" s="18"/>
     </row>
     <row r="559">
-      <c r="B559" s="17"/>
+      <c r="B559" s="18"/>
     </row>
     <row r="560">
-      <c r="B560" s="17"/>
+      <c r="B560" s="18"/>
     </row>
     <row r="561">
-      <c r="B561" s="17"/>
+      <c r="B561" s="18"/>
     </row>
     <row r="562">
-      <c r="B562" s="17"/>
+      <c r="B562" s="18"/>
     </row>
     <row r="563">
-      <c r="B563" s="17"/>
+      <c r="B563" s="18"/>
     </row>
     <row r="564">
-      <c r="B564" s="17"/>
+      <c r="B564" s="18"/>
     </row>
     <row r="565">
-      <c r="B565" s="17"/>
+      <c r="B565" s="18"/>
     </row>
     <row r="566">
-      <c r="B566" s="17"/>
+      <c r="B566" s="18"/>
     </row>
     <row r="567">
-      <c r="B567" s="17"/>
+      <c r="B567" s="18"/>
     </row>
     <row r="568">
-      <c r="B568" s="17"/>
+      <c r="B568" s="18"/>
     </row>
     <row r="569">
-      <c r="B569" s="17"/>
+      <c r="B569" s="18"/>
     </row>
     <row r="570">
-      <c r="B570" s="17"/>
+      <c r="B570" s="18"/>
     </row>
     <row r="571">
-      <c r="B571" s="17"/>
+      <c r="B571" s="18"/>
     </row>
     <row r="572">
-      <c r="B572" s="17"/>
+      <c r="B572" s="18"/>
     </row>
     <row r="573">
-      <c r="B573" s="17"/>
+      <c r="B573" s="18"/>
     </row>
     <row r="574">
-      <c r="B574" s="17"/>
+      <c r="B574" s="18"/>
     </row>
     <row r="575">
-      <c r="B575" s="17"/>
+      <c r="B575" s="18"/>
     </row>
     <row r="576">
-      <c r="B576" s="17"/>
+      <c r="B576" s="18"/>
     </row>
     <row r="577">
-      <c r="B577" s="17"/>
+      <c r="B577" s="18"/>
     </row>
     <row r="578">
-      <c r="B578" s="17"/>
+      <c r="B578" s="18"/>
     </row>
     <row r="579">
-      <c r="B579" s="17"/>
+      <c r="B579" s="18"/>
     </row>
     <row r="580">
-      <c r="B580" s="17"/>
+      <c r="B580" s="18"/>
     </row>
     <row r="581">
-      <c r="B581" s="17"/>
+      <c r="B581" s="18"/>
     </row>
     <row r="582">
-      <c r="B582" s="17"/>
+      <c r="B582" s="18"/>
     </row>
     <row r="583">
-      <c r="B583" s="17"/>
+      <c r="B583" s="18"/>
     </row>
     <row r="584">
-      <c r="B584" s="17"/>
+      <c r="B584" s="18"/>
     </row>
     <row r="585">
-      <c r="B585" s="17"/>
+      <c r="B585" s="18"/>
     </row>
     <row r="586">
-      <c r="B586" s="17"/>
+      <c r="B586" s="18"/>
     </row>
     <row r="587">
-      <c r="B587" s="17"/>
+      <c r="B587" s="18"/>
     </row>
     <row r="588">
-      <c r="B588" s="17"/>
+      <c r="B588" s="18"/>
     </row>
     <row r="589">
-      <c r="B589" s="17"/>
+      <c r="B589" s="18"/>
     </row>
     <row r="590">
-      <c r="B590" s="17"/>
+      <c r="B590" s="18"/>
     </row>
     <row r="591">
-      <c r="B591" s="17"/>
+      <c r="B591" s="18"/>
     </row>
     <row r="592">
-      <c r="B592" s="17"/>
+      <c r="B592" s="18"/>
     </row>
     <row r="593">
-      <c r="B593" s="17"/>
+      <c r="B593" s="18"/>
     </row>
     <row r="594">
-      <c r="B594" s="17"/>
+      <c r="B594" s="18"/>
     </row>
     <row r="595">
-      <c r="B595" s="17"/>
+      <c r="B595" s="18"/>
     </row>
     <row r="596">
-      <c r="B596" s="17"/>
+      <c r="B596" s="18"/>
     </row>
     <row r="597">
-      <c r="B597" s="17"/>
+      <c r="B597" s="18"/>
     </row>
     <row r="598">
-      <c r="B598" s="17"/>
+      <c r="B598" s="18"/>
     </row>
     <row r="599">
-      <c r="B599" s="17"/>
+      <c r="B599" s="18"/>
     </row>
     <row r="600">
-      <c r="B600" s="17"/>
+      <c r="B600" s="18"/>
     </row>
     <row r="601">
-      <c r="B601" s="17"/>
+      <c r="B601" s="18"/>
     </row>
     <row r="602">
-      <c r="B602" s="17"/>
+      <c r="B602" s="18"/>
     </row>
     <row r="603">
-      <c r="B603" s="17"/>
+      <c r="B603" s="18"/>
     </row>
     <row r="604">
-      <c r="B604" s="17"/>
+      <c r="B604" s="18"/>
     </row>
     <row r="605">
-      <c r="B605" s="17"/>
+      <c r="B605" s="18"/>
     </row>
     <row r="606">
-      <c r="B606" s="17"/>
+      <c r="B606" s="18"/>
     </row>
     <row r="607">
-      <c r="B607" s="17"/>
+      <c r="B607" s="18"/>
     </row>
     <row r="608">
-      <c r="B608" s="17"/>
+      <c r="B608" s="18"/>
     </row>
     <row r="609">
-      <c r="B609" s="17"/>
+      <c r="B609" s="18"/>
     </row>
     <row r="610">
-      <c r="B610" s="17"/>
+      <c r="B610" s="18"/>
     </row>
     <row r="611">
-      <c r="B611" s="17"/>
+      <c r="B611" s="18"/>
     </row>
     <row r="612">
-      <c r="B612" s="17"/>
+      <c r="B612" s="18"/>
     </row>
     <row r="613">
-      <c r="B613" s="17"/>
+      <c r="B613" s="18"/>
     </row>
     <row r="614">
-      <c r="B614" s="17"/>
+      <c r="B614" s="18"/>
     </row>
     <row r="615">
-      <c r="B615" s="17"/>
+      <c r="B615" s="18"/>
     </row>
     <row r="616">
-      <c r="B616" s="17"/>
+      <c r="B616" s="18"/>
     </row>
     <row r="617">
-      <c r="B617" s="17"/>
+      <c r="B617" s="18"/>
     </row>
     <row r="618">
-      <c r="B618" s="17"/>
+      <c r="B618" s="18"/>
     </row>
     <row r="619">
-      <c r="B619" s="17"/>
+      <c r="B619" s="18"/>
     </row>
     <row r="620">
-      <c r="B620" s="17"/>
+      <c r="B620" s="18"/>
     </row>
     <row r="621">
-      <c r="B621" s="17"/>
+      <c r="B621" s="18"/>
     </row>
     <row r="622">
-      <c r="B622" s="17"/>
+      <c r="B622" s="18"/>
     </row>
     <row r="623">
-      <c r="B623" s="17"/>
+      <c r="B623" s="18"/>
     </row>
     <row r="624">
-      <c r="B624" s="17"/>
+      <c r="B624" s="18"/>
     </row>
     <row r="625">
-      <c r="B625" s="17"/>
+      <c r="B625" s="18"/>
     </row>
     <row r="626">
-      <c r="B626" s="17"/>
+      <c r="B626" s="18"/>
     </row>
     <row r="627">
-      <c r="B627" s="17"/>
+      <c r="B627" s="18"/>
     </row>
     <row r="628">
-      <c r="B628" s="17"/>
+      <c r="B628" s="18"/>
     </row>
     <row r="629">
-      <c r="B629" s="17"/>
+      <c r="B629" s="18"/>
     </row>
     <row r="630">
-      <c r="B630" s="17"/>
+      <c r="B630" s="18"/>
     </row>
     <row r="631">
-      <c r="B631" s="17"/>
+      <c r="B631" s="18"/>
     </row>
     <row r="632">
-      <c r="B632" s="17"/>
+      <c r="B632" s="18"/>
     </row>
     <row r="633">
-      <c r="B633" s="17"/>
+      <c r="B633" s="18"/>
     </row>
     <row r="634">
-      <c r="B634" s="17"/>
+      <c r="B634" s="18"/>
     </row>
     <row r="635">
-      <c r="B635" s="17"/>
+      <c r="B635" s="18"/>
     </row>
     <row r="636">
-      <c r="B636" s="17"/>
+      <c r="B636" s="18"/>
     </row>
     <row r="637">
-      <c r="B637" s="17"/>
+      <c r="B637" s="18"/>
     </row>
     <row r="638">
-      <c r="B638" s="17"/>
+      <c r="B638" s="18"/>
     </row>
     <row r="639">
-      <c r="B639" s="17"/>
+      <c r="B639" s="18"/>
     </row>
     <row r="640">
-      <c r="B640" s="17"/>
+      <c r="B640" s="18"/>
     </row>
     <row r="641">
-      <c r="B641" s="17"/>
+      <c r="B641" s="18"/>
     </row>
     <row r="642">
-      <c r="B642" s="17"/>
+      <c r="B642" s="18"/>
     </row>
     <row r="643">
-      <c r="B643" s="17"/>
+      <c r="B643" s="18"/>
     </row>
     <row r="644">
-      <c r="B644" s="17"/>
+      <c r="B644" s="18"/>
     </row>
     <row r="645">
-      <c r="B645" s="17"/>
+      <c r="B645" s="18"/>
     </row>
     <row r="646">
-      <c r="B646" s="17"/>
+      <c r="B646" s="18"/>
     </row>
     <row r="647">
-      <c r="B647" s="17"/>
+      <c r="B647" s="18"/>
     </row>
     <row r="648">
-      <c r="B648" s="17"/>
+      <c r="B648" s="18"/>
     </row>
     <row r="649">
-      <c r="B649" s="17"/>
+      <c r="B649" s="18"/>
     </row>
     <row r="650">
-      <c r="B650" s="17"/>
+      <c r="B650" s="18"/>
     </row>
     <row r="651">
-      <c r="B651" s="17"/>
+      <c r="B651" s="18"/>
     </row>
     <row r="652">
-      <c r="B652" s="17"/>
+      <c r="B652" s="18"/>
     </row>
     <row r="653">
-      <c r="B653" s="17"/>
+      <c r="B653" s="18"/>
     </row>
     <row r="654">
-      <c r="B654" s="17"/>
+      <c r="B654" s="18"/>
     </row>
     <row r="655">
-      <c r="B655" s="17"/>
+      <c r="B655" s="18"/>
     </row>
     <row r="656">
-      <c r="B656" s="17"/>
+      <c r="B656" s="18"/>
     </row>
     <row r="657">
-      <c r="B657" s="17"/>
+      <c r="B657" s="18"/>
     </row>
     <row r="658">
-      <c r="B658" s="17"/>
+      <c r="B658" s="18"/>
     </row>
     <row r="659">
-      <c r="B659" s="17"/>
+      <c r="B659" s="18"/>
     </row>
     <row r="660">
-      <c r="B660" s="17"/>
+      <c r="B660" s="18"/>
     </row>
     <row r="661">
-      <c r="B661" s="17"/>
+      <c r="B661" s="18"/>
     </row>
     <row r="662">
-      <c r="B662" s="17"/>
+      <c r="B662" s="18"/>
     </row>
     <row r="663">
-      <c r="B663" s="17"/>
+      <c r="B663" s="18"/>
     </row>
     <row r="664">
-      <c r="B664" s="17"/>
+      <c r="B664" s="18"/>
     </row>
     <row r="665">
-      <c r="B665" s="17"/>
+      <c r="B665" s="18"/>
     </row>
     <row r="666">
-      <c r="B666" s="17"/>
+      <c r="B666" s="18"/>
     </row>
     <row r="667">
-      <c r="B667" s="17"/>
+      <c r="B667" s="18"/>
     </row>
     <row r="668">
-      <c r="B668" s="17"/>
+      <c r="B668" s="18"/>
     </row>
     <row r="669">
-      <c r="B669" s="17"/>
+      <c r="B669" s="18"/>
     </row>
     <row r="670">
-      <c r="B670" s="17"/>
+      <c r="B670" s="18"/>
     </row>
     <row r="671">
-      <c r="B671" s="17"/>
+      <c r="B671" s="18"/>
     </row>
     <row r="672">
-      <c r="B672" s="17"/>
+      <c r="B672" s="18"/>
     </row>
     <row r="673">
-      <c r="B673" s="17"/>
+      <c r="B673" s="18"/>
     </row>
     <row r="674">
-      <c r="B674" s="17"/>
+      <c r="B674" s="18"/>
     </row>
     <row r="675">
-      <c r="B675" s="17"/>
+      <c r="B675" s="18"/>
     </row>
     <row r="676">
-      <c r="B676" s="17"/>
+      <c r="B676" s="18"/>
     </row>
     <row r="677">
-      <c r="B677" s="17"/>
+      <c r="B677" s="18"/>
     </row>
     <row r="678">
-      <c r="B678" s="17"/>
+      <c r="B678" s="18"/>
     </row>
     <row r="679">
-      <c r="B679" s="17"/>
+      <c r="B679" s="18"/>
     </row>
     <row r="680">
-      <c r="B680" s="17"/>
+      <c r="B680" s="18"/>
     </row>
     <row r="681">
-      <c r="B681" s="17"/>
+      <c r="B681" s="18"/>
     </row>
     <row r="682">
-      <c r="B682" s="17"/>
+      <c r="B682" s="18"/>
     </row>
     <row r="683">
-      <c r="B683" s="17"/>
+      <c r="B683" s="18"/>
     </row>
     <row r="684">
-      <c r="B684" s="17"/>
+      <c r="B684" s="18"/>
     </row>
     <row r="685">
-      <c r="B685" s="17"/>
+      <c r="B685" s="18"/>
     </row>
     <row r="686">
-      <c r="B686" s="17"/>
+      <c r="B686" s="18"/>
     </row>
     <row r="687">
-      <c r="B687" s="17"/>
+      <c r="B687" s="18"/>
     </row>
     <row r="688">
-      <c r="B688" s="17"/>
+      <c r="B688" s="18"/>
     </row>
     <row r="689">
-      <c r="B689" s="17"/>
+      <c r="B689" s="18"/>
     </row>
     <row r="690">
-      <c r="B690" s="17"/>
+      <c r="B690" s="18"/>
     </row>
     <row r="691">
-      <c r="B691" s="17"/>
+      <c r="B691" s="18"/>
     </row>
     <row r="692">
-      <c r="B692" s="17"/>
+      <c r="B692" s="18"/>
     </row>
     <row r="693">
-      <c r="B693" s="17"/>
+      <c r="B693" s="18"/>
     </row>
     <row r="694">
-      <c r="B694" s="17"/>
+      <c r="B694" s="18"/>
     </row>
     <row r="695">
-      <c r="B695" s="17"/>
+      <c r="B695" s="18"/>
     </row>
     <row r="696">
-      <c r="B696" s="17"/>
+      <c r="B696" s="18"/>
     </row>
     <row r="697">
-      <c r="B697" s="17"/>
+      <c r="B697" s="18"/>
     </row>
     <row r="698">
-      <c r="B698" s="17"/>
+      <c r="B698" s="18"/>
     </row>
     <row r="699">
-      <c r="B699" s="17"/>
+      <c r="B699" s="18"/>
     </row>
     <row r="700">
-      <c r="B700" s="17"/>
+      <c r="B700" s="18"/>
     </row>
     <row r="701">
-      <c r="B701" s="17"/>
+      <c r="B701" s="18"/>
     </row>
     <row r="702">
-      <c r="B702" s="17"/>
+      <c r="B702" s="18"/>
     </row>
     <row r="703">
-      <c r="B703" s="17"/>
+      <c r="B703" s="18"/>
     </row>
     <row r="704">
-      <c r="B704" s="17"/>
+      <c r="B704" s="18"/>
     </row>
     <row r="705">
-      <c r="B705" s="17"/>
+      <c r="B705" s="18"/>
     </row>
     <row r="706">
-      <c r="B706" s="17"/>
+      <c r="B706" s="18"/>
     </row>
     <row r="707">
-      <c r="B707" s="17"/>
+      <c r="B707" s="18"/>
     </row>
     <row r="708">
-      <c r="B708" s="17"/>
+      <c r="B708" s="18"/>
     </row>
     <row r="709">
-      <c r="B709" s="17"/>
+      <c r="B709" s="18"/>
     </row>
     <row r="710">
-      <c r="B710" s="17"/>
+      <c r="B710" s="18"/>
     </row>
     <row r="711">
-      <c r="B711" s="17"/>
+      <c r="B711" s="18"/>
     </row>
     <row r="712">
-      <c r="B712" s="17"/>
+      <c r="B712" s="18"/>
     </row>
     <row r="713">
-      <c r="B713" s="17"/>
+      <c r="B713" s="18"/>
     </row>
     <row r="714">
-      <c r="B714" s="17"/>
+      <c r="B714" s="18"/>
     </row>
     <row r="715">
-      <c r="B715" s="17"/>
+      <c r="B715" s="18"/>
     </row>
     <row r="716">
-      <c r="B716" s="17"/>
+      <c r="B716" s="18"/>
     </row>
     <row r="717">
-      <c r="B717" s="17"/>
+      <c r="B717" s="18"/>
     </row>
     <row r="718">
-      <c r="B718" s="17"/>
+      <c r="B718" s="18"/>
     </row>
     <row r="719">
-      <c r="B719" s="17"/>
+      <c r="B719" s="18"/>
     </row>
     <row r="720">
-      <c r="B720" s="17"/>
+      <c r="B720" s="18"/>
     </row>
     <row r="721">
-      <c r="B721" s="17"/>
+      <c r="B721" s="18"/>
     </row>
     <row r="722">
-      <c r="B722" s="17"/>
+      <c r="B722" s="18"/>
     </row>
     <row r="723">
-      <c r="B723" s="17"/>
+      <c r="B723" s="18"/>
     </row>
     <row r="724">
-      <c r="B724" s="17"/>
+      <c r="B724" s="18"/>
     </row>
     <row r="725">
-      <c r="B725" s="17"/>
+      <c r="B725" s="18"/>
     </row>
     <row r="726">
-      <c r="B726" s="17"/>
+      <c r="B726" s="18"/>
     </row>
     <row r="727">
-      <c r="B727" s="17"/>
+      <c r="B727" s="18"/>
     </row>
     <row r="728">
-      <c r="B728" s="17"/>
+      <c r="B728" s="18"/>
     </row>
     <row r="729">
-      <c r="B729" s="17"/>
+      <c r="B729" s="18"/>
     </row>
     <row r="730">
-      <c r="B730" s="17"/>
+      <c r="B730" s="18"/>
     </row>
     <row r="731">
-      <c r="B731" s="17"/>
+      <c r="B731" s="18"/>
     </row>
     <row r="732">
-      <c r="B732" s="17"/>
+      <c r="B732" s="18"/>
     </row>
     <row r="733">
-      <c r="B733" s="17"/>
+      <c r="B733" s="18"/>
     </row>
     <row r="734">
-      <c r="B734" s="17"/>
+      <c r="B734" s="18"/>
     </row>
     <row r="735">
-      <c r="B735" s="17"/>
+      <c r="B735" s="18"/>
     </row>
     <row r="736">
-      <c r="B736" s="17"/>
+      <c r="B736" s="18"/>
     </row>
     <row r="737">
-      <c r="B737" s="17"/>
+      <c r="B737" s="18"/>
     </row>
     <row r="738">
-      <c r="B738" s="17"/>
+      <c r="B738" s="18"/>
     </row>
     <row r="739">
-      <c r="B739" s="17"/>
+      <c r="B739" s="18"/>
     </row>
     <row r="740">
-      <c r="B740" s="17"/>
+      <c r="B740" s="18"/>
     </row>
     <row r="741">
-      <c r="B741" s="17"/>
+      <c r="B741" s="18"/>
     </row>
     <row r="742">
-      <c r="B742" s="17"/>
+      <c r="B742" s="18"/>
     </row>
     <row r="743">
-      <c r="B743" s="17"/>
+      <c r="B743" s="18"/>
     </row>
     <row r="744">
-      <c r="B744" s="17"/>
+      <c r="B744" s="18"/>
     </row>
     <row r="745">
-      <c r="B745" s="17"/>
+      <c r="B745" s="18"/>
     </row>
     <row r="746">
-      <c r="B746" s="17"/>
+      <c r="B746" s="18"/>
     </row>
     <row r="747">
-      <c r="B747" s="17"/>
+      <c r="B747" s="18"/>
     </row>
     <row r="748">
-      <c r="B748" s="17"/>
+      <c r="B748" s="18"/>
     </row>
     <row r="749">
-      <c r="B749" s="17"/>
+      <c r="B749" s="18"/>
     </row>
     <row r="750">
-      <c r="B750" s="17"/>
+      <c r="B750" s="18"/>
     </row>
     <row r="751">
-      <c r="B751" s="17"/>
+      <c r="B751" s="18"/>
     </row>
     <row r="752">
-      <c r="B752" s="17"/>
+      <c r="B752" s="18"/>
     </row>
     <row r="753">
-      <c r="B753" s="17"/>
+      <c r="B753" s="18"/>
     </row>
     <row r="754">
-      <c r="B754" s="17"/>
+      <c r="B754" s="18"/>
     </row>
     <row r="755">
-      <c r="B755" s="17"/>
+      <c r="B755" s="18"/>
     </row>
     <row r="756">
-      <c r="B756" s="17"/>
+      <c r="B756" s="18"/>
     </row>
     <row r="757">
-      <c r="B757" s="17"/>
+      <c r="B757" s="18"/>
     </row>
     <row r="758">
-      <c r="B758" s="17"/>
+      <c r="B758" s="18"/>
     </row>
     <row r="759">
-      <c r="B759" s="17"/>
+      <c r="B759" s="18"/>
     </row>
     <row r="760">
-      <c r="B760" s="17"/>
+      <c r="B760" s="18"/>
     </row>
     <row r="761">
-      <c r="B761" s="17"/>
+      <c r="B761" s="18"/>
     </row>
     <row r="762">
-      <c r="B762" s="17"/>
+      <c r="B762" s="18"/>
     </row>
     <row r="763">
-      <c r="B763" s="17"/>
+      <c r="B763" s="18"/>
     </row>
     <row r="764">
-      <c r="B764" s="17"/>
+      <c r="B764" s="18"/>
     </row>
     <row r="765">
-      <c r="B765" s="17"/>
+      <c r="B765" s="18"/>
     </row>
     <row r="766">
-      <c r="B766" s="17"/>
+      <c r="B766" s="18"/>
     </row>
     <row r="767">
-      <c r="B767" s="17"/>
+      <c r="B767" s="18"/>
     </row>
     <row r="768">
-      <c r="B768" s="17"/>
+      <c r="B768" s="18"/>
     </row>
     <row r="769">
-      <c r="B769" s="17"/>
+      <c r="B769" s="18"/>
     </row>
     <row r="770">
-      <c r="B770" s="17"/>
+      <c r="B770" s="18"/>
     </row>
     <row r="771">
-      <c r="B771" s="17"/>
+      <c r="B771" s="18"/>
     </row>
     <row r="772">
-      <c r="B772" s="17"/>
+      <c r="B772" s="18"/>
     </row>
     <row r="773">
-      <c r="B773" s="17"/>
+      <c r="B773" s="18"/>
     </row>
     <row r="774">
-      <c r="B774" s="17"/>
+      <c r="B774" s="18"/>
     </row>
     <row r="775">
-      <c r="B775" s="17"/>
+      <c r="B775" s="18"/>
     </row>
     <row r="776">
-      <c r="B776" s="17"/>
+      <c r="B776" s="18"/>
     </row>
     <row r="777">
-      <c r="B777" s="17"/>
+      <c r="B777" s="18"/>
     </row>
     <row r="778">
-      <c r="B778" s="17"/>
+      <c r="B778" s="18"/>
     </row>
     <row r="779">
-      <c r="B779" s="17"/>
+      <c r="B779" s="18"/>
     </row>
     <row r="780">
-      <c r="B780" s="17"/>
+      <c r="B780" s="18"/>
     </row>
     <row r="781">
-      <c r="B781" s="17"/>
+      <c r="B781" s="18"/>
     </row>
     <row r="782">
-      <c r="B782" s="17"/>
+      <c r="B782" s="18"/>
     </row>
     <row r="783">
-      <c r="B783" s="17"/>
+      <c r="B783" s="18"/>
     </row>
     <row r="784">
-      <c r="B784" s="17"/>
+      <c r="B784" s="18"/>
     </row>
     <row r="785">
-      <c r="B785" s="17"/>
+      <c r="B785" s="18"/>
     </row>
     <row r="786">
-      <c r="B786" s="17"/>
+      <c r="B786" s="18"/>
     </row>
     <row r="787">
-      <c r="B787" s="17"/>
+      <c r="B787" s="18"/>
     </row>
     <row r="788">
-      <c r="B788" s="17"/>
+      <c r="B788" s="18"/>
     </row>
     <row r="789">
-      <c r="B789" s="17"/>
+      <c r="B789" s="18"/>
     </row>
     <row r="790">
-      <c r="B790" s="17"/>
+      <c r="B790" s="18"/>
     </row>
     <row r="791">
-      <c r="B791" s="17"/>
+      <c r="B791" s="18"/>
     </row>
     <row r="792">
-      <c r="B792" s="17"/>
+      <c r="B792" s="18"/>
     </row>
     <row r="793">
-      <c r="B793" s="17"/>
+      <c r="B793" s="18"/>
     </row>
     <row r="794">
-      <c r="B794" s="17"/>
+      <c r="B794" s="18"/>
     </row>
     <row r="795">
-      <c r="B795" s="17"/>
+      <c r="B795" s="18"/>
     </row>
     <row r="796">
-      <c r="B796" s="17"/>
+      <c r="B796" s="18"/>
     </row>
     <row r="797">
-      <c r="B797" s="17"/>
+      <c r="B797" s="18"/>
     </row>
     <row r="798">
-      <c r="B798" s="17"/>
+      <c r="B798" s="18"/>
     </row>
     <row r="799">
-      <c r="B799" s="17"/>
+      <c r="B799" s="18"/>
     </row>
     <row r="800">
-      <c r="B800" s="17"/>
+      <c r="B800" s="18"/>
     </row>
     <row r="801">
-      <c r="B801" s="17"/>
+      <c r="B801" s="18"/>
     </row>
     <row r="802">
-      <c r="B802" s="17"/>
+      <c r="B802" s="18"/>
     </row>
     <row r="803">
-      <c r="B803" s="17"/>
+      <c r="B803" s="18"/>
     </row>
     <row r="804">
-      <c r="B804" s="17"/>
+      <c r="B804" s="18"/>
     </row>
     <row r="805">
-      <c r="B805" s="17"/>
+      <c r="B805" s="18"/>
     </row>
     <row r="806">
-      <c r="B806" s="17"/>
+      <c r="B806" s="18"/>
     </row>
     <row r="807">
-      <c r="B807" s="17"/>
+      <c r="B807" s="18"/>
     </row>
     <row r="808">
-      <c r="B808" s="17"/>
+      <c r="B808" s="18"/>
     </row>
     <row r="809">
-      <c r="B809" s="17"/>
+      <c r="B809" s="18"/>
     </row>
     <row r="810">
-      <c r="B810" s="17"/>
+      <c r="B810" s="18"/>
     </row>
     <row r="811">
-      <c r="B811" s="17"/>
+      <c r="B811" s="18"/>
     </row>
     <row r="812">
-      <c r="B812" s="17"/>
+      <c r="B812" s="18"/>
     </row>
     <row r="813">
-      <c r="B813" s="17"/>
+      <c r="B813" s="18"/>
     </row>
     <row r="814">
-      <c r="B814" s="17"/>
+      <c r="B814" s="18"/>
     </row>
     <row r="815">
-      <c r="B815" s="17"/>
+      <c r="B815" s="18"/>
     </row>
     <row r="816">
-      <c r="B816" s="17"/>
+      <c r="B816" s="18"/>
     </row>
     <row r="817">
-      <c r="B817" s="17"/>
+      <c r="B817" s="18"/>
     </row>
     <row r="818">
-      <c r="B818" s="17"/>
+      <c r="B818" s="18"/>
     </row>
     <row r="819">
-      <c r="B819" s="17"/>
+      <c r="B819" s="18"/>
     </row>
     <row r="820">
-      <c r="B820" s="17"/>
+      <c r="B820" s="18"/>
     </row>
     <row r="821">
-      <c r="B821" s="17"/>
+      <c r="B821" s="18"/>
     </row>
     <row r="822">
-      <c r="B822" s="17"/>
+      <c r="B822" s="18"/>
     </row>
     <row r="823">
-      <c r="B823" s="17"/>
+      <c r="B823" s="18"/>
     </row>
     <row r="824">
-      <c r="B824" s="17"/>
+      <c r="B824" s="18"/>
     </row>
     <row r="825">
-      <c r="B825" s="17"/>
+      <c r="B825" s="18"/>
     </row>
     <row r="826">
-      <c r="B826" s="17"/>
+      <c r="B826" s="18"/>
     </row>
     <row r="827">
-      <c r="B827" s="17"/>
+      <c r="B827" s="18"/>
     </row>
     <row r="828">
-      <c r="B828" s="17"/>
+      <c r="B828" s="18"/>
     </row>
     <row r="829">
-      <c r="B829" s="17"/>
+      <c r="B829" s="18"/>
     </row>
     <row r="830">
-      <c r="B830" s="17"/>
+      <c r="B830" s="18"/>
     </row>
     <row r="831">
-      <c r="B831" s="17"/>
+      <c r="B831" s="18"/>
     </row>
     <row r="832">
-      <c r="B832" s="17"/>
+      <c r="B832" s="18"/>
     </row>
     <row r="833">
-      <c r="B833" s="17"/>
+      <c r="B833" s="18"/>
     </row>
     <row r="834">
-      <c r="B834" s="17"/>
+      <c r="B834" s="18"/>
     </row>
     <row r="835">
-      <c r="B835" s="17"/>
+      <c r="B835" s="18"/>
     </row>
     <row r="836">
-      <c r="B836" s="17"/>
+      <c r="B836" s="18"/>
     </row>
     <row r="837">
-      <c r="B837" s="17"/>
+      <c r="B837" s="18"/>
     </row>
     <row r="838">
-      <c r="B838" s="17"/>
+      <c r="B838" s="18"/>
     </row>
     <row r="839">
-      <c r="B839" s="17"/>
+      <c r="B839" s="18"/>
     </row>
     <row r="840">
-      <c r="B840" s="17"/>
+      <c r="B840" s="18"/>
     </row>
     <row r="841">
-      <c r="B841" s="17"/>
+      <c r="B841" s="18"/>
     </row>
     <row r="842">
-      <c r="B842" s="17"/>
+      <c r="B842" s="18"/>
     </row>
     <row r="843">
-      <c r="B843" s="17"/>
+      <c r="B843" s="18"/>
     </row>
     <row r="844">
-      <c r="B844" s="17"/>
+      <c r="B844" s="18"/>
     </row>
     <row r="845">
-      <c r="B845" s="17"/>
+      <c r="B845" s="18"/>
     </row>
     <row r="846">
-      <c r="B846" s="17"/>
+      <c r="B846" s="18"/>
     </row>
     <row r="847">
-      <c r="B847" s="17"/>
+      <c r="B847" s="18"/>
     </row>
     <row r="848">
-      <c r="B848" s="17"/>
+      <c r="B848" s="18"/>
     </row>
     <row r="849">
-      <c r="B849" s="17"/>
+      <c r="B849" s="18"/>
     </row>
     <row r="850">
-      <c r="B850" s="17"/>
+      <c r="B850" s="18"/>
     </row>
     <row r="851">
-      <c r="B851" s="17"/>
+      <c r="B851" s="18"/>
     </row>
     <row r="852">
-      <c r="B852" s="17"/>
+      <c r="B852" s="18"/>
     </row>
     <row r="853">
-      <c r="B853" s="17"/>
+      <c r="B853" s="18"/>
     </row>
     <row r="854">
-      <c r="B854" s="17"/>
+      <c r="B854" s="18"/>
     </row>
     <row r="855">
-      <c r="B855" s="17"/>
+      <c r="B855" s="18"/>
     </row>
     <row r="856">
-      <c r="B856" s="17"/>
+      <c r="B856" s="18"/>
     </row>
     <row r="857">
-      <c r="B857" s="17"/>
+      <c r="B857" s="18"/>
     </row>
     <row r="858">
-      <c r="B858" s="17"/>
+      <c r="B858" s="18"/>
     </row>
     <row r="859">
-      <c r="B859" s="17"/>
+      <c r="B859" s="18"/>
     </row>
     <row r="860">
-      <c r="B860" s="17"/>
+      <c r="B860" s="18"/>
     </row>
     <row r="861">
-      <c r="B861" s="17"/>
+      <c r="B861" s="18"/>
     </row>
     <row r="862">
-      <c r="B862" s="17"/>
+      <c r="B862" s="18"/>
     </row>
     <row r="863">
-      <c r="B863" s="17"/>
+      <c r="B863" s="18"/>
     </row>
     <row r="864">
-      <c r="B864" s="17"/>
+      <c r="B864" s="18"/>
     </row>
     <row r="865">
-      <c r="B865" s="17"/>
+      <c r="B865" s="18"/>
     </row>
     <row r="866">
-      <c r="B866" s="17"/>
+      <c r="B866" s="18"/>
     </row>
     <row r="867">
-      <c r="B867" s="17"/>
+      <c r="B867" s="18"/>
     </row>
     <row r="868">
-      <c r="B868" s="17"/>
+      <c r="B868" s="18"/>
     </row>
     <row r="869">
-      <c r="B869" s="17"/>
+      <c r="B869" s="18"/>
     </row>
     <row r="870">
-      <c r="B870" s="17"/>
+      <c r="B870" s="18"/>
     </row>
     <row r="871">
-      <c r="B871" s="17"/>
+      <c r="B871" s="18"/>
     </row>
     <row r="872">
-      <c r="B872" s="17"/>
+      <c r="B872" s="18"/>
     </row>
     <row r="873">
-      <c r="B873" s="17"/>
+      <c r="B873" s="18"/>
     </row>
     <row r="874">
-      <c r="B874" s="17"/>
+      <c r="B874" s="18"/>
     </row>
     <row r="875">
-      <c r="B875" s="17"/>
+      <c r="B875" s="18"/>
     </row>
     <row r="876">
-      <c r="B876" s="17"/>
+      <c r="B876" s="18"/>
     </row>
     <row r="877">
-      <c r="B877" s="17"/>
+      <c r="B877" s="18"/>
     </row>
     <row r="878">
-      <c r="B878" s="17"/>
+      <c r="B878" s="18"/>
     </row>
     <row r="879">
-      <c r="B879" s="17"/>
+      <c r="B879" s="18"/>
     </row>
     <row r="880">
-      <c r="B880" s="17"/>
+      <c r="B880" s="18"/>
     </row>
     <row r="881">
-      <c r="B881" s="17"/>
+      <c r="B881" s="18"/>
     </row>
     <row r="882">
-      <c r="B882" s="17"/>
+      <c r="B882" s="18"/>
     </row>
     <row r="883">
-      <c r="B883" s="17"/>
+      <c r="B883" s="18"/>
     </row>
     <row r="884">
-      <c r="B884" s="17"/>
+      <c r="B884" s="18"/>
     </row>
     <row r="885">
-      <c r="B885" s="17"/>
+      <c r="B885" s="18"/>
     </row>
     <row r="886">
-      <c r="B886" s="17"/>
+      <c r="B886" s="18"/>
     </row>
     <row r="887">
-      <c r="B887" s="17"/>
+      <c r="B887" s="18"/>
     </row>
     <row r="888">
-      <c r="B888" s="17"/>
+      <c r="B888" s="18"/>
     </row>
     <row r="889">
-      <c r="B889" s="17"/>
+      <c r="B889" s="18"/>
     </row>
     <row r="890">
-      <c r="B890" s="17"/>
+      <c r="B890" s="18"/>
     </row>
     <row r="891">
-      <c r="B891" s="17"/>
+      <c r="B891" s="18"/>
     </row>
     <row r="892">
-      <c r="B892" s="17"/>
+      <c r="B892" s="18"/>
     </row>
     <row r="893">
-      <c r="B893" s="17"/>
+      <c r="B893" s="18"/>
     </row>
     <row r="894">
-      <c r="B894" s="17"/>
+      <c r="B894" s="18"/>
     </row>
     <row r="895">
-      <c r="B895" s="17"/>
+      <c r="B895" s="18"/>
     </row>
     <row r="896">
-      <c r="B896" s="17"/>
+      <c r="B896" s="18"/>
     </row>
     <row r="897">
-      <c r="B897" s="17"/>
+      <c r="B897" s="18"/>
     </row>
     <row r="898">
-      <c r="B898" s="17"/>
+      <c r="B898" s="18"/>
     </row>
     <row r="899">
-      <c r="B899" s="17"/>
+      <c r="B899" s="18"/>
     </row>
     <row r="900">
-      <c r="B900" s="17"/>
+      <c r="B900" s="18"/>
     </row>
     <row r="901">
-      <c r="B901" s="17"/>
+      <c r="B901" s="18"/>
     </row>
     <row r="902">
-      <c r="B902" s="17"/>
+      <c r="B902" s="18"/>
     </row>
     <row r="903">
-      <c r="B903" s="17"/>
+      <c r="B903" s="18"/>
     </row>
     <row r="904">
-      <c r="B904" s="17"/>
+      <c r="B904" s="18"/>
     </row>
     <row r="905">
-      <c r="B905" s="17"/>
+      <c r="B905" s="18"/>
     </row>
     <row r="906">
-      <c r="B906" s="17"/>
+      <c r="B906" s="18"/>
     </row>
     <row r="907">
-      <c r="B907" s="17"/>
+      <c r="B907" s="18"/>
     </row>
     <row r="908">
-      <c r="B908" s="17"/>
+      <c r="B908" s="18"/>
     </row>
     <row r="909">
-      <c r="B909" s="17"/>
+      <c r="B909" s="18"/>
     </row>
     <row r="910">
-      <c r="B910" s="17"/>
+      <c r="B910" s="18"/>
     </row>
     <row r="911">
-      <c r="B911" s="17"/>
+      <c r="B911" s="18"/>
     </row>
     <row r="912">
-      <c r="B912" s="17"/>
+      <c r="B912" s="18"/>
     </row>
     <row r="913">
-      <c r="B913" s="17"/>
+      <c r="B913" s="18"/>
     </row>
     <row r="914">
-      <c r="B914" s="17"/>
+      <c r="B914" s="18"/>
     </row>
     <row r="915">
-      <c r="B915" s="17"/>
+      <c r="B915" s="18"/>
     </row>
     <row r="916">
-      <c r="B916" s="17"/>
+      <c r="B916" s="18"/>
     </row>
     <row r="917">
-      <c r="B917" s="17"/>
+      <c r="B917" s="18"/>
     </row>
     <row r="918">
-      <c r="B918" s="17"/>
+      <c r="B918" s="18"/>
     </row>
     <row r="919">
-      <c r="B919" s="17"/>
+      <c r="B919" s="18"/>
     </row>
     <row r="920">
-      <c r="B920" s="17"/>
+      <c r="B920" s="18"/>
     </row>
     <row r="921">
-      <c r="B921" s="17"/>
+      <c r="B921" s="18"/>
     </row>
     <row r="922">
-      <c r="B922" s="17"/>
+      <c r="B922" s="18"/>
     </row>
     <row r="923">
-      <c r="B923" s="17"/>
+      <c r="B923" s="18"/>
     </row>
     <row r="924">
-      <c r="B924" s="17"/>
+      <c r="B924" s="18"/>
     </row>
     <row r="925">
-      <c r="B925" s="17"/>
+      <c r="B925" s="18"/>
     </row>
     <row r="926">
-      <c r="B926" s="17"/>
+      <c r="B926" s="18"/>
     </row>
     <row r="927">
-      <c r="B927" s="17"/>
+      <c r="B927" s="18"/>
     </row>
     <row r="928">
-      <c r="B928" s="17"/>
+      <c r="B928" s="18"/>
     </row>
     <row r="929">
-      <c r="B929" s="17"/>
+      <c r="B929" s="18"/>
     </row>
     <row r="930">
-      <c r="B930" s="17"/>
+      <c r="B930" s="18"/>
     </row>
     <row r="931">
-      <c r="B931" s="17"/>
+      <c r="B931" s="18"/>
     </row>
     <row r="932">
-      <c r="B932" s="17"/>
+      <c r="B932" s="18"/>
     </row>
     <row r="933">
-      <c r="B933" s="17"/>
+      <c r="B933" s="18"/>
     </row>
     <row r="934">
-      <c r="B934" s="17"/>
+      <c r="B934" s="18"/>
     </row>
     <row r="935">
-      <c r="B935" s="17"/>
+      <c r="B935" s="18"/>
     </row>
     <row r="936">
-      <c r="B936" s="17"/>
+      <c r="B936" s="18"/>
     </row>
     <row r="937">
-      <c r="B937" s="17"/>
+      <c r="B937" s="18"/>
     </row>
     <row r="938">
-      <c r="B938" s="17"/>
+      <c r="B938" s="18"/>
     </row>
     <row r="939">
-      <c r="B939" s="17"/>
+      <c r="B939" s="18"/>
     </row>
     <row r="940">
-      <c r="B940" s="17"/>
+      <c r="B940" s="18"/>
     </row>
     <row r="941">
-      <c r="B941" s="17"/>
+      <c r="B941" s="18"/>
     </row>
     <row r="942">
-      <c r="B942" s="17"/>
+      <c r="B942" s="18"/>
     </row>
     <row r="943">
-      <c r="B943" s="17"/>
+      <c r="B943" s="18"/>
     </row>
     <row r="944">
-      <c r="B944" s="17"/>
+      <c r="B944" s="18"/>
     </row>
     <row r="945">
-      <c r="B945" s="17"/>
+      <c r="B945" s="18"/>
     </row>
     <row r="946">
-      <c r="B946" s="17"/>
+      <c r="B946" s="18"/>
     </row>
     <row r="947">
-      <c r="B947" s="17"/>
+      <c r="B947" s="18"/>
     </row>
     <row r="948">
-      <c r="B948" s="17"/>
+      <c r="B948" s="18"/>
     </row>
     <row r="949">
-      <c r="B949" s="17"/>
+      <c r="B949" s="18"/>
     </row>
     <row r="950">
-      <c r="B950" s="17"/>
+      <c r="B950" s="18"/>
     </row>
     <row r="951">
-      <c r="B951" s="17"/>
+      <c r="B951" s="18"/>
     </row>
     <row r="952">
-      <c r="B952" s="17"/>
+      <c r="B952" s="18"/>
     </row>
     <row r="953">
-      <c r="B953" s="17"/>
+      <c r="B953" s="18"/>
     </row>
     <row r="954">
-      <c r="B954" s="17"/>
+      <c r="B954" s="18"/>
     </row>
     <row r="955">
-      <c r="B955" s="17"/>
+      <c r="B955" s="18"/>
     </row>
     <row r="956">
-      <c r="B956" s="17"/>
+      <c r="B956" s="18"/>
     </row>
     <row r="957">
-      <c r="B957" s="17"/>
+      <c r="B957" s="18"/>
     </row>
     <row r="958">
-      <c r="B958" s="17"/>
+      <c r="B958" s="18"/>
     </row>
     <row r="959">
-      <c r="B959" s="17"/>
+      <c r="B959" s="18"/>
     </row>
     <row r="960">
-      <c r="B960" s="17"/>
+      <c r="B960" s="18"/>
     </row>
     <row r="961">
-      <c r="B961" s="17"/>
+      <c r="B961" s="18"/>
     </row>
     <row r="962">
-      <c r="B962" s="17"/>
+      <c r="B962" s="18"/>
     </row>
     <row r="963">
-      <c r="B963" s="17"/>
+      <c r="B963" s="18"/>
     </row>
     <row r="964">
-      <c r="B964" s="17"/>
+      <c r="B964" s="18"/>
     </row>
     <row r="965">
-      <c r="B965" s="17"/>
+      <c r="B965" s="18"/>
     </row>
     <row r="966">
-      <c r="B966" s="17"/>
+      <c r="B966" s="18"/>
     </row>
     <row r="967">
-      <c r="B967" s="17"/>
+      <c r="B967" s="18"/>
     </row>
     <row r="968">
-      <c r="B968" s="17"/>
+      <c r="B968" s="18"/>
     </row>
     <row r="969">
-      <c r="B969" s="17"/>
+      <c r="B969" s="18"/>
     </row>
     <row r="970">
-      <c r="B970" s="17"/>
+      <c r="B970" s="18"/>
     </row>
     <row r="971">
-      <c r="B971" s="17"/>
+      <c r="B971" s="18"/>
     </row>
     <row r="972">
-      <c r="B972" s="17"/>
+      <c r="B972" s="18"/>
     </row>
     <row r="973">
-      <c r="B973" s="17"/>
+      <c r="B973" s="18"/>
     </row>
     <row r="974">
-      <c r="B974" s="17"/>
+      <c r="B974" s="18"/>
     </row>
     <row r="975">
-      <c r="B975" s="17"/>
+      <c r="B975" s="18"/>
     </row>
     <row r="976">
-      <c r="B976" s="17"/>
+      <c r="B976" s="18"/>
     </row>
     <row r="977">
-      <c r="B977" s="17"/>
+      <c r="B977" s="18"/>
     </row>
     <row r="978">
-      <c r="B978" s="17"/>
+      <c r="B978" s="18"/>
     </row>
     <row r="979">
-      <c r="B979" s="17"/>
+      <c r="B979" s="18"/>
     </row>
     <row r="980">
-      <c r="B980" s="17"/>
+      <c r="B980" s="18"/>
     </row>
     <row r="981">
-      <c r="B981" s="17"/>
+      <c r="B981" s="18"/>
     </row>
     <row r="982">
-      <c r="B982" s="17"/>
+      <c r="B982" s="18"/>
     </row>
     <row r="983">
-      <c r="B983" s="17"/>
+      <c r="B983" s="18"/>
     </row>
     <row r="984">
-      <c r="B984" s="17"/>
+      <c r="B984" s="18"/>
     </row>
     <row r="985">
-      <c r="B985" s="17"/>
+      <c r="B985" s="18"/>
     </row>
     <row r="986">
-      <c r="B986" s="17"/>
+      <c r="B986" s="18"/>
     </row>
     <row r="987">
-      <c r="B987" s="17"/>
+      <c r="B987" s="18"/>
     </row>
     <row r="988">
-      <c r="B988" s="17"/>
+      <c r="B988" s="18"/>
     </row>
     <row r="989">
-      <c r="B989" s="17"/>
+      <c r="B989" s="18"/>
     </row>
     <row r="990">
-      <c r="B990" s="17"/>
+      <c r="B990" s="18"/>
     </row>
     <row r="991">
-      <c r="B991" s="17"/>
+      <c r="B991" s="18"/>
     </row>
     <row r="992">
-      <c r="B992" s="17"/>
+      <c r="B992" s="18"/>
     </row>
     <row r="993">
-      <c r="B993" s="17"/>
+      <c r="B993" s="18"/>
     </row>
     <row r="994">
-      <c r="B994" s="17"/>
+      <c r="B994" s="18"/>
     </row>
     <row r="995">
-      <c r="B995" s="17"/>
+      <c r="B995" s="18"/>
     </row>
     <row r="996">
-      <c r="B996" s="17"/>
+      <c r="B996" s="18"/>
     </row>
     <row r="997">
-      <c r="B997" s="17"/>
+      <c r="B997" s="18"/>
     </row>
     <row r="998">
-      <c r="B998" s="17"/>
+      <c r="B998" s="18"/>
     </row>
     <row r="999">
-      <c r="B999" s="17"/>
+      <c r="B999" s="18"/>
     </row>
     <row r="1000">
-      <c r="B1000" s="17"/>
+      <c r="B1000" s="18"/>
     </row>
     <row r="1001">
-      <c r="B1001" s="17"/>
+      <c r="B1001" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="D1:F1"/>
   </mergeCells>
-  <drawing r:id="rId1"/>
+  <hyperlinks>
+    <hyperlink r:id="rId1" ref="D19"/>
+    <hyperlink r:id="rId2" ref="G28"/>
+  </hyperlinks>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>